<commit_message>
Modify initial pension income process
-Replace lagged gross income covariate with lagged level of potential hourly wages
</commit_message>
<xml_diff>
--- a/input/reg_income.xlsx
+++ b/input/reg_income.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46C2927-D3B6-44EA-9F95-619D741F1DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BAB749-E613-49AC-9C37-B9A8896CB82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" tabRatio="852" firstSheet="5" activeTab="11" xr2:uid="{8DDB884B-4CBA-4D96-8159-4841B9678181}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="852" firstSheet="5" activeTab="10" xr2:uid="{8DDB884B-4CBA-4D96-8159-4841B9678181}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="7" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="147">
   <si>
     <t>REGRESSOR</t>
   </si>
@@ -495,6 +495,9 @@
   </si>
   <si>
     <t>RealGDPGrowth</t>
+  </si>
+  <si>
+    <t>L1_hourly_wage</t>
   </si>
 </sst>
 </file>
@@ -3579,9 +3582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42C8444-64E3-46A6-8707-99C15C89A426}">
   <dimension ref="A1:Y24"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:Y1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3621,7 +3622,7 @@
         <v>85</v>
       </c>
       <c r="K1" t="s">
-        <v>106</v>
+        <v>146</v>
       </c>
       <c r="L1" t="s">
         <v>87</v>
@@ -3671,76 +3672,76 @@
         <v>144</v>
       </c>
       <c r="B2" s="28">
-        <v>0.25753721615794484</v>
+        <v>0.13937490191697868</v>
       </c>
       <c r="C2">
-        <v>5.95714656141349E-2</v>
+        <v>9.1862140648868898E-2</v>
       </c>
       <c r="D2">
-        <v>-2.7580335854844934E-3</v>
+        <v>-7.9061866869369422E-3</v>
       </c>
       <c r="E2">
-        <v>-4.4227528951094972E-3</v>
+        <v>-7.6928622118868743E-3</v>
       </c>
       <c r="F2">
-        <v>-3.0101553470160913E-2</v>
+        <v>-2.4779614956179204E-2</v>
       </c>
       <c r="G2">
-        <v>6.7477969627558233E-3</v>
+        <v>6.0695273194271843E-3</v>
       </c>
       <c r="H2">
-        <v>1.7381987922607299E-4</v>
+        <v>-4.1923419036085843E-3</v>
       </c>
       <c r="I2">
-        <v>1.8975326102572201E-3</v>
+        <v>1.799529418391177E-3</v>
       </c>
       <c r="J2">
-        <v>-1.7588914427196412E-3</v>
+        <v>-2.0351395561085932E-3</v>
       </c>
       <c r="K2">
-        <v>2.5282097216740018E-3</v>
+        <v>-9.9183961826385467E-5</v>
       </c>
       <c r="L2">
-        <v>1.3291230667013067E-2</v>
+        <v>1.436046278028795E-2</v>
       </c>
       <c r="M2">
-        <v>4.5163068018624162E-3</v>
+        <v>6.9220679436423418E-3</v>
       </c>
       <c r="N2">
-        <v>1.036561008173428E-2</v>
+        <v>1.7451689890816746E-2</v>
       </c>
       <c r="O2">
-        <v>8.270172876976678E-3</v>
+        <v>1.4440825791191339E-2</v>
       </c>
       <c r="P2">
-        <v>3.6326346137162159E-3</v>
+        <v>5.6513204836884101E-3</v>
       </c>
       <c r="Q2">
-        <v>4.6511656485942153E-3</v>
+        <v>1.9766776784912593E-3</v>
       </c>
       <c r="R2">
-        <v>3.9272257873377067E-3</v>
+        <v>4.6846492494128228E-3</v>
       </c>
       <c r="S2">
-        <v>9.0164703008346822E-3</v>
+        <v>1.2686614753749284E-2</v>
       </c>
       <c r="T2">
-        <v>4.677629974442446E-3</v>
+        <v>1.0761750685467711E-2</v>
       </c>
       <c r="U2">
-        <v>1.7802789660290051E-2</v>
+        <v>3.0078683257696727E-2</v>
       </c>
       <c r="V2">
-        <v>6.3206753664585905E-3</v>
+        <v>9.23838811834507E-3</v>
       </c>
       <c r="W2">
-        <v>-0.12859751300421518</v>
+        <v>-0.49909184781068894</v>
       </c>
       <c r="X2">
-        <v>1.2878847130870961E-3</v>
+        <v>9.4308232184674781E-3</v>
       </c>
       <c r="Y2">
-        <v>0.10062466744780638</v>
+        <v>0.35850112933657174</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -3748,76 +3749,76 @@
         <v>99</v>
       </c>
       <c r="B3" s="28">
-        <v>-0.86485191616799995</v>
+        <v>-0.81850665132027145</v>
       </c>
       <c r="C3">
-        <v>-2.7580335854844934E-3</v>
+        <v>-7.9061866869369422E-3</v>
       </c>
       <c r="D3">
-        <v>6.7934379003829606E-2</v>
+        <v>8.5973446120168939E-2</v>
       </c>
       <c r="E3">
-        <v>4.6421772920972541E-2</v>
+        <v>5.9410821672562106E-2</v>
       </c>
       <c r="F3">
-        <v>4.9245247403055491E-3</v>
+        <v>3.5420279590641429E-3</v>
       </c>
       <c r="G3">
-        <v>1.1734401520416271E-3</v>
+        <v>7.7628755574513306E-3</v>
       </c>
       <c r="H3">
-        <v>-3.9909542875011623E-3</v>
+        <v>-4.2892696443911707E-3</v>
       </c>
       <c r="I3">
-        <v>6.4661463639600555E-3</v>
+        <v>2.4009107249805914E-2</v>
       </c>
       <c r="J3">
-        <v>1.9464818209498774E-3</v>
+        <v>1.9240519982464538E-3</v>
       </c>
       <c r="K3">
-        <v>2.4138049156638972E-4</v>
+        <v>3.4033318043258549E-4</v>
       </c>
       <c r="L3">
-        <v>-1.4012202193975212E-2</v>
+        <v>-1.4077473347480204E-2</v>
       </c>
       <c r="M3">
-        <v>-1.0930141029429716E-2</v>
+        <v>-1.0904699692027738E-2</v>
       </c>
       <c r="N3">
-        <v>-8.1863878695853168E-3</v>
+        <v>-8.937408573629943E-3</v>
       </c>
       <c r="O3">
-        <v>-1.6046243935155365E-2</v>
+        <v>-1.4597769225485474E-2</v>
       </c>
       <c r="P3">
-        <v>-2.8788524312352917E-3</v>
+        <v>-5.6020297237818761E-4</v>
       </c>
       <c r="Q3">
-        <v>-8.2247944361459879E-3</v>
+        <v>-6.2085119454594606E-3</v>
       </c>
       <c r="R3">
-        <v>-1.2361470457209763E-2</v>
+        <v>-1.6382424858995062E-2</v>
       </c>
       <c r="S3">
-        <v>-1.136685627626529E-2</v>
+        <v>-1.1485756972139591E-2</v>
       </c>
       <c r="T3">
-        <v>-1.4576270915288583E-2</v>
+        <v>-1.7701984247219638E-2</v>
       </c>
       <c r="U3">
-        <v>-2.0700040476634624E-2</v>
+        <v>-2.5915912104090617E-2</v>
       </c>
       <c r="V3">
-        <v>-1.1480691743811389E-2</v>
+        <v>-1.2049797758661496E-2</v>
       </c>
       <c r="W3">
-        <v>0.1770734298214712</v>
+        <v>0.30259720862195666</v>
       </c>
       <c r="X3">
-        <v>-3.5638620644135198E-3</v>
+        <v>-5.8798245187188123E-3</v>
       </c>
       <c r="Y3">
-        <v>-0.16574530152585606</v>
+        <v>-0.26976885796582967</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -3825,76 +3826,76 @@
         <v>100</v>
       </c>
       <c r="B4" s="28">
-        <v>-1.9339962881601449</v>
+        <v>-1.7517111220985719</v>
       </c>
       <c r="C4">
-        <v>-4.4227528951094972E-3</v>
+        <v>-7.6928622118868743E-3</v>
       </c>
       <c r="D4">
-        <v>4.6421772920972541E-2</v>
+        <v>5.9410821672562106E-2</v>
       </c>
       <c r="E4">
-        <v>8.299459518203739E-2</v>
+        <v>0.11140390576527447</v>
       </c>
       <c r="F4">
-        <v>5.169303678367332E-3</v>
+        <v>1.135454725083479E-2</v>
       </c>
       <c r="G4">
-        <v>7.8636206533017096E-3</v>
+        <v>1.831049072014505E-2</v>
       </c>
       <c r="H4">
-        <v>-1.5275680196849394E-3</v>
+        <v>3.6402034133134302E-5</v>
       </c>
       <c r="I4">
-        <v>1.0756345666420621E-2</v>
+        <v>8.9310152661675295E-3</v>
       </c>
       <c r="J4">
-        <v>4.383797119618219E-3</v>
+        <v>4.7068017580606161E-3</v>
       </c>
       <c r="K4">
-        <v>1.1884124322444727E-3</v>
+        <v>4.3175630681401581E-4</v>
       </c>
       <c r="L4">
-        <v>-5.9197976887454609E-3</v>
+        <v>4.6984751753052084E-4</v>
       </c>
       <c r="M4">
-        <v>-1.9273324511565292E-3</v>
+        <v>4.0110970870882411E-3</v>
       </c>
       <c r="N4">
-        <v>1.73419599372171E-3</v>
+        <v>5.0878896610192341E-3</v>
       </c>
       <c r="O4">
-        <v>-3.3167244440372723E-3</v>
+        <v>5.2441726494273158E-3</v>
       </c>
       <c r="P4">
-        <v>1.7582866181414109E-4</v>
+        <v>6.0858907004433943E-3</v>
       </c>
       <c r="Q4">
-        <v>2.6732900577197682E-4</v>
+        <v>1.0366089694286873E-2</v>
       </c>
       <c r="R4">
-        <v>8.5844585569955917E-4</v>
+        <v>5.2912155902574247E-3</v>
       </c>
       <c r="S4">
-        <v>-1.4058153812108454E-3</v>
+        <v>5.5514772783760852E-3</v>
       </c>
       <c r="T4">
-        <v>-7.890926965583106E-3</v>
+        <v>-4.6745526778994434E-3</v>
       </c>
       <c r="U4">
-        <v>-9.9409563042813995E-3</v>
+        <v>-8.8346045426468747E-3</v>
       </c>
       <c r="V4">
-        <v>-7.4874865499970356E-3</v>
+        <v>3.2369187177399145E-3</v>
       </c>
       <c r="W4">
-        <v>6.2142406410686524E-3</v>
+        <v>0.17187058027941179</v>
       </c>
       <c r="X4">
-        <v>6.7409750167927432E-4</v>
+        <v>-3.0855420892277148E-3</v>
       </c>
       <c r="Y4">
-        <v>-8.186503916477611E-2</v>
+        <v>-0.21544635656109054</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -3902,76 +3903,76 @@
         <v>139</v>
       </c>
       <c r="B5" s="28">
-        <v>0.84800121888354163</v>
+        <v>1.2502156169531469</v>
       </c>
       <c r="C5">
-        <v>-3.0101553470160913E-2</v>
+        <v>-2.4779614956179204E-2</v>
       </c>
       <c r="D5">
-        <v>4.9245247403055491E-3</v>
+        <v>3.5420279590641429E-3</v>
       </c>
       <c r="E5">
-        <v>5.169303678367332E-3</v>
+        <v>1.135454725083479E-2</v>
       </c>
       <c r="F5">
-        <v>0.21848457869027135</v>
+        <v>8.5231401434311765E-2</v>
       </c>
       <c r="G5">
-        <v>1.6670223793524352E-2</v>
+        <v>2.9348963488305714E-3</v>
       </c>
       <c r="H5">
-        <v>6.2692776348592123E-3</v>
+        <v>8.8833477883090983E-3</v>
       </c>
       <c r="I5">
-        <v>2.8817017051284734E-2</v>
+        <v>1.2914076460165558E-2</v>
       </c>
       <c r="J5">
-        <v>-6.4393283714407491E-3</v>
+        <v>-9.6065904693438398E-3</v>
       </c>
       <c r="K5">
-        <v>-2.1758463596310555E-2</v>
+        <v>-2.4504356561933562E-4</v>
       </c>
       <c r="L5">
-        <v>-5.2250514042813858E-3</v>
+        <v>-9.4476862386802651E-3</v>
       </c>
       <c r="M5">
-        <v>-2.2954173392850073E-3</v>
+        <v>-4.5815373878275341E-3</v>
       </c>
       <c r="N5">
-        <v>-6.6196711599207803E-3</v>
+        <v>-1.1717316561958518E-2</v>
       </c>
       <c r="O5">
-        <v>-5.9571927191093207E-3</v>
+        <v>-1.6600383072309089E-2</v>
       </c>
       <c r="P5">
-        <v>2.9973889028888333E-4</v>
+        <v>-1.1956730471953461E-2</v>
       </c>
       <c r="Q5">
-        <v>-7.9732776127569259E-3</v>
+        <v>-6.6405122162020956E-3</v>
       </c>
       <c r="R5">
-        <v>-1.0658843709390076E-2</v>
+        <v>-7.9437022184900979E-3</v>
       </c>
       <c r="S5">
-        <v>-9.3217748714856039E-3</v>
+        <v>-1.1219747640836412E-2</v>
       </c>
       <c r="T5">
-        <v>-6.3383861452735828E-3</v>
+        <v>-9.9687609496605708E-3</v>
       </c>
       <c r="U5">
-        <v>-2.7404599490629573E-3</v>
+        <v>-8.4462357562314939E-3</v>
       </c>
       <c r="V5">
-        <v>-6.8614152929517072E-3</v>
+        <v>2.3106493170582665E-5</v>
       </c>
       <c r="W5">
-        <v>-9.4748967033658829E-3</v>
+        <v>-3.7449364467653252E-3</v>
       </c>
       <c r="X5">
-        <v>-4.3509181755516579E-4</v>
+        <v>-2.5863207909175687E-4</v>
       </c>
       <c r="Y5">
-        <v>6.1738594960714238E-3</v>
+        <v>-1.169781030315196E-2</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -3979,76 +3980,76 @@
         <v>103</v>
       </c>
       <c r="B6" s="28">
-        <v>-0.485422663849228</v>
+        <v>-0.17757928971163472</v>
       </c>
       <c r="C6">
-        <v>6.7477969627558233E-3</v>
+        <v>6.0695273194271843E-3</v>
       </c>
       <c r="D6">
-        <v>1.1734401520416271E-3</v>
+        <v>7.7628755574513306E-3</v>
       </c>
       <c r="E6">
-        <v>7.8636206533017096E-3</v>
+        <v>1.831049072014505E-2</v>
       </c>
       <c r="F6">
-        <v>1.6670223793524352E-2</v>
+        <v>2.9348963488305714E-3</v>
       </c>
       <c r="G6">
-        <v>0.28335114311260234</v>
+        <v>0.33692562321296532</v>
       </c>
       <c r="H6">
-        <v>1.5400257600742633E-2</v>
+        <v>1.8955002492610527E-2</v>
       </c>
       <c r="I6">
-        <v>2.5637537968523673E-2</v>
+        <v>3.3092128997953024E-2</v>
       </c>
       <c r="J6">
-        <v>-4.6234977210094994E-4</v>
+        <v>-1.566573674745303E-3</v>
       </c>
       <c r="K6">
-        <v>-1.59244555982373E-3</v>
+        <v>1.8669213344427675E-4</v>
       </c>
       <c r="L6">
-        <v>2.0618087830267945E-3</v>
+        <v>8.8025159127544939E-3</v>
       </c>
       <c r="M6">
-        <v>1.1507578069408494E-2</v>
+        <v>1.495913678547614E-2</v>
       </c>
       <c r="N6">
-        <v>3.8319754585348503E-3</v>
+        <v>6.0664421063431201E-3</v>
       </c>
       <c r="O6">
-        <v>7.5495253552309571E-3</v>
+        <v>1.6070337363201723E-2</v>
       </c>
       <c r="P6">
-        <v>2.1976760475354851E-3</v>
+        <v>1.0705885560449435E-2</v>
       </c>
       <c r="Q6">
-        <v>8.0673847068077967E-3</v>
+        <v>1.7384254433432625E-2</v>
       </c>
       <c r="R6">
-        <v>2.6863390895296373E-2</v>
+        <v>3.8423704110529359E-2</v>
       </c>
       <c r="S6">
-        <v>2.1122285969539918E-2</v>
+        <v>3.2754378936420261E-2</v>
       </c>
       <c r="T6">
-        <v>1.1381805881844204E-2</v>
+        <v>2.6220920390710695E-2</v>
       </c>
       <c r="U6">
-        <v>1.4355189390636861E-2</v>
+        <v>2.3804769729267136E-2</v>
       </c>
       <c r="V6">
-        <v>6.2169779290617289E-3</v>
+        <v>1.2762979654432599E-2</v>
       </c>
       <c r="W6">
-        <v>0.44835790866042852</v>
+        <v>0.67520338388582224</v>
       </c>
       <c r="X6">
-        <v>-9.0805752208120514E-3</v>
+        <v>-1.2753389154642867E-2</v>
       </c>
       <c r="Y6">
-        <v>-0.34254788914150153</v>
+        <v>-0.52783804092838593</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -4056,76 +4057,76 @@
         <v>104</v>
       </c>
       <c r="B7" s="28">
-        <v>-0.25816687297316837</v>
+        <v>-0.1885988581669136</v>
       </c>
       <c r="C7">
-        <v>1.7381987922607299E-4</v>
+        <v>-4.1923419036085843E-3</v>
       </c>
       <c r="D7">
-        <v>-3.9909542875011623E-3</v>
+        <v>-4.2892696443911707E-3</v>
       </c>
       <c r="E7">
-        <v>-1.5275680196849394E-3</v>
+        <v>3.6402034133134302E-5</v>
       </c>
       <c r="F7">
-        <v>6.2692776348592123E-3</v>
+        <v>8.8833477883090983E-3</v>
       </c>
       <c r="G7">
-        <v>1.5400257600742633E-2</v>
+        <v>1.8955002492610527E-2</v>
       </c>
       <c r="H7">
-        <v>5.4044603082643243E-2</v>
+        <v>7.0481104217524751E-2</v>
       </c>
       <c r="I7">
-        <v>1.6102586656290909E-2</v>
+        <v>1.7250902446205474E-2</v>
       </c>
       <c r="J7">
-        <v>1.3670514360807915E-3</v>
+        <v>2.6004084854767025E-3</v>
       </c>
       <c r="K7">
-        <v>2.2783173732603091E-4</v>
+        <v>6.6725617321959077E-5</v>
       </c>
       <c r="L7">
-        <v>-1.6316119816999625E-3</v>
+        <v>-1.0435350534517135E-2</v>
       </c>
       <c r="M7">
-        <v>-1.3148131155760676E-3</v>
+        <v>-8.6671329194928717E-3</v>
       </c>
       <c r="N7">
-        <v>-2.8539887751991705E-4</v>
+        <v>-5.2898114164224297E-3</v>
       </c>
       <c r="O7">
-        <v>1.1583515079843926E-3</v>
+        <v>-2.2404681610428967E-3</v>
       </c>
       <c r="P7">
-        <v>2.4397538701321914E-3</v>
+        <v>-2.8561636157380249E-3</v>
       </c>
       <c r="Q7">
-        <v>1.0944915455193931E-3</v>
+        <v>-1.531864003406741E-3</v>
       </c>
       <c r="R7">
-        <v>2.4723807910925419E-3</v>
+        <v>-2.4729128864216798E-3</v>
       </c>
       <c r="S7">
-        <v>2.218659369730442E-3</v>
+        <v>9.2166909737528835E-4</v>
       </c>
       <c r="T7">
-        <v>5.0724609843613572E-3</v>
+        <v>2.5447735050496134E-4</v>
       </c>
       <c r="U7">
-        <v>6.3329104904553297E-3</v>
+        <v>5.1830568021328516E-3</v>
       </c>
       <c r="V7">
-        <v>-5.386090787335443E-3</v>
+        <v>-7.8847001118066973E-3</v>
       </c>
       <c r="W7">
-        <v>0.16581199600601518</v>
+        <v>0.19026725533048905</v>
       </c>
       <c r="X7">
-        <v>-3.7589510799761962E-3</v>
+        <v>-4.427860264708228E-3</v>
       </c>
       <c r="Y7">
-        <v>-0.13297975441268098</v>
+        <v>-0.15299354988962166</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -4133,76 +4134,76 @@
         <v>105</v>
       </c>
       <c r="B8" s="28">
-        <v>-1.8626388218328325</v>
+        <v>-1.4347390865986227</v>
       </c>
       <c r="C8">
-        <v>1.8975326102572201E-3</v>
+        <v>1.799529418391177E-3</v>
       </c>
       <c r="D8">
-        <v>6.4661463639600555E-3</v>
+        <v>2.4009107249805914E-2</v>
       </c>
       <c r="E8">
-        <v>1.0756345666420621E-2</v>
+        <v>8.9310152661675295E-3</v>
       </c>
       <c r="F8">
-        <v>2.8817017051284734E-2</v>
+        <v>1.2914076460165558E-2</v>
       </c>
       <c r="G8">
-        <v>2.5637537968523673E-2</v>
+        <v>3.3092128997953024E-2</v>
       </c>
       <c r="H8">
-        <v>1.6102586656290909E-2</v>
+        <v>1.7250902446205474E-2</v>
       </c>
       <c r="I8">
-        <v>2.2301798586705326</v>
+        <v>2.928368377690755</v>
       </c>
       <c r="J8">
-        <v>1.5292724507459318E-3</v>
+        <v>-7.8510610699686137E-3</v>
       </c>
       <c r="K8">
-        <v>-2.8247914836934296E-3</v>
+        <v>1.679347105639555E-4</v>
       </c>
       <c r="L8">
-        <v>3.7872386698837496E-2</v>
+        <v>6.3549667420949807E-2</v>
       </c>
       <c r="M8">
-        <v>1.1919966010008595E-2</v>
+        <v>2.6150067191342219E-2</v>
       </c>
       <c r="N8">
-        <v>-2.6637954924914609E-3</v>
+        <v>6.7453252365120953E-2</v>
       </c>
       <c r="O8">
-        <v>3.9275171997395331E-2</v>
+        <v>6.2961990483366981E-2</v>
       </c>
       <c r="P8">
-        <v>4.0937706280476521E-2</v>
+        <v>7.0303442078546108E-2</v>
       </c>
       <c r="Q8">
-        <v>4.2429339555317164E-2</v>
+        <v>5.3631581734316036E-2</v>
       </c>
       <c r="R8">
-        <v>3.9718345080824641E-2</v>
+        <v>6.4125504081869567E-2</v>
       </c>
       <c r="S8">
-        <v>4.1173819527528743E-2</v>
+        <v>6.8856750884901341E-2</v>
       </c>
       <c r="T8">
-        <v>1.9657391728534201E-2</v>
+        <v>2.7564447175786766E-2</v>
       </c>
       <c r="U8">
-        <v>4.3251802117939608E-2</v>
+        <v>6.9694960238182668E-2</v>
       </c>
       <c r="V8">
-        <v>3.7901231694003723E-2</v>
+        <v>6.8159608276641359E-2</v>
       </c>
       <c r="W8">
-        <v>0.80297652089649851</v>
+        <v>1.243657955007619</v>
       </c>
       <c r="X8">
-        <v>-1.6209879001932173E-2</v>
+        <v>-2.4206046454630925E-2</v>
       </c>
       <c r="Y8">
-        <v>-0.61752305240079197</v>
+        <v>-0.94747786620384689</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -4210,153 +4211,153 @@
         <v>85</v>
       </c>
       <c r="B9" s="28">
-        <v>0.20591378836965996</v>
+        <v>0.19260116839801417</v>
       </c>
       <c r="C9">
-        <v>-1.7588914427196412E-3</v>
+        <v>-2.0351395561085932E-3</v>
       </c>
       <c r="D9">
-        <v>1.9464818209498774E-3</v>
+        <v>1.9240519982464538E-3</v>
       </c>
       <c r="E9">
-        <v>4.383797119618219E-3</v>
+        <v>4.7068017580606161E-3</v>
       </c>
       <c r="F9">
-        <v>-6.4393283714407491E-3</v>
+        <v>-9.6065904693438398E-3</v>
       </c>
       <c r="G9">
-        <v>-4.6234977210094994E-4</v>
+        <v>-1.566573674745303E-3</v>
       </c>
       <c r="H9">
-        <v>1.3670514360807915E-3</v>
+        <v>2.6004084854767025E-3</v>
       </c>
       <c r="I9">
-        <v>1.5292724507459318E-3</v>
+        <v>-7.8510610699686137E-3</v>
       </c>
       <c r="J9">
-        <v>8.7182223289109378E-3</v>
+        <v>1.170069625934644E-2</v>
       </c>
       <c r="K9">
-        <v>-2.4752202335701946E-4</v>
+        <v>-4.5379425153057007E-5</v>
       </c>
       <c r="L9">
-        <v>1.2956087926007387E-3</v>
+        <v>-1.8884763082885753E-3</v>
       </c>
       <c r="M9">
-        <v>1.9824519917849264E-3</v>
+        <v>9.6499460693572417E-4</v>
       </c>
       <c r="N9">
-        <v>-3.0333166376464091E-4</v>
+        <v>-1.7803044128895246E-3</v>
       </c>
       <c r="O9">
-        <v>1.0888739948411164E-3</v>
+        <v>2.2445298234975639E-3</v>
       </c>
       <c r="P9">
-        <v>-4.5297912090492068E-4</v>
+        <v>-1.3761566682159027E-3</v>
       </c>
       <c r="Q9">
-        <v>1.4143056169158182E-3</v>
+        <v>2.2121249963394374E-4</v>
       </c>
       <c r="R9">
-        <v>3.354013412493825E-3</v>
+        <v>2.8940153707164608E-3</v>
       </c>
       <c r="S9">
-        <v>1.1557299792795024E-3</v>
+        <v>1.9301016037318944E-3</v>
       </c>
       <c r="T9">
-        <v>9.1289437508450255E-4</v>
+        <v>-1.1267893663378242E-3</v>
       </c>
       <c r="U9">
-        <v>-1.2741078469166167E-3</v>
+        <v>-2.8450322456401028E-3</v>
       </c>
       <c r="V9">
-        <v>1.5356764501257836E-3</v>
+        <v>-1.2180361960801023E-3</v>
       </c>
       <c r="W9">
-        <v>9.732603082362172E-2</v>
+        <v>0.1487602517616321</v>
       </c>
       <c r="X9">
-        <v>-2.2591520193440697E-3</v>
+        <v>-3.5649193954222919E-3</v>
       </c>
       <c r="Y9">
-        <v>-8.7895924857041868E-2</v>
+        <v>-0.1270444315462424</v>
       </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>146</v>
       </c>
       <c r="B10" s="28">
-        <v>7.1518872395938071E-2</v>
+        <v>1.8893364253986839E-3</v>
       </c>
       <c r="C10">
-        <v>2.5282097216740018E-3</v>
+        <v>-9.9183961826385467E-5</v>
       </c>
       <c r="D10">
-        <v>2.4138049156638972E-4</v>
+        <v>3.4033318043258549E-4</v>
       </c>
       <c r="E10">
-        <v>1.1884124322444727E-3</v>
+        <v>4.3175630681401581E-4</v>
       </c>
       <c r="F10">
-        <v>-2.1758463596310555E-2</v>
+        <v>-2.4504356561933562E-4</v>
       </c>
       <c r="G10">
-        <v>-1.59244555982373E-3</v>
+        <v>1.8669213344427675E-4</v>
       </c>
       <c r="H10">
-        <v>2.2783173732603091E-4</v>
+        <v>6.6725617321959077E-5</v>
       </c>
       <c r="I10">
-        <v>-2.8247914836934296E-3</v>
+        <v>1.679347105639555E-4</v>
       </c>
       <c r="J10">
-        <v>-2.4752202335701946E-4</v>
+        <v>-4.5379425153057007E-5</v>
       </c>
       <c r="K10">
-        <v>2.9959543346597551E-3</v>
+        <v>2.5003937521954629E-5</v>
       </c>
       <c r="L10">
-        <v>-5.0724779235327084E-4</v>
+        <v>9.939072593046435E-5</v>
       </c>
       <c r="M10">
-        <v>-4.7866177210160966E-5</v>
+        <v>8.3501032164255592E-5</v>
       </c>
       <c r="N10">
-        <v>2.7249314730435053E-4</v>
+        <v>8.8745004312389521E-5</v>
       </c>
       <c r="O10">
-        <v>-1.0779516239298311E-4</v>
+        <v>6.9153602464497297E-5</v>
       </c>
       <c r="P10">
-        <v>-1.0186499461616767E-3</v>
+        <v>1.0561772035569227E-4</v>
       </c>
       <c r="Q10">
-        <v>8.6987516164464644E-5</v>
+        <v>1.2934305696620874E-4</v>
       </c>
       <c r="R10">
-        <v>4.6777039952655523E-4</v>
+        <v>1.8961697431795946E-5</v>
       </c>
       <c r="S10">
-        <v>2.8249183400097175E-4</v>
+        <v>8.1360577123522007E-5</v>
       </c>
       <c r="T10">
-        <v>5.768544494111922E-4</v>
+        <v>8.6534115583630241E-5</v>
       </c>
       <c r="U10">
-        <v>-3.3581427123569908E-4</v>
+        <v>-1.9968931484756918E-5</v>
       </c>
       <c r="V10">
-        <v>6.4430694030079803E-4</v>
+        <v>1.5171193759525069E-4</v>
       </c>
       <c r="W10">
-        <v>4.3378494090640981E-3</v>
+        <v>-1.1724764118938046E-3</v>
       </c>
       <c r="X10">
-        <v>-5.9376932972964031E-5</v>
+        <v>2.4345436624344039E-5</v>
       </c>
       <c r="Y10">
-        <v>-4.3345736870255723E-3</v>
+        <v>3.3640744664203092E-4</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -4364,76 +4365,76 @@
         <v>87</v>
       </c>
       <c r="B11" s="28">
-        <v>0.13222441515260436</v>
+        <v>0.63583086716133286</v>
       </c>
       <c r="C11">
-        <v>1.3291230667013067E-2</v>
+        <v>1.436046278028795E-2</v>
       </c>
       <c r="D11">
-        <v>-1.4012202193975212E-2</v>
+        <v>-1.4077473347480204E-2</v>
       </c>
       <c r="E11">
-        <v>-5.9197976887454609E-3</v>
+        <v>4.6984751753052084E-4</v>
       </c>
       <c r="F11">
-        <v>-5.2250514042813858E-3</v>
+        <v>-9.4476862386802651E-3</v>
       </c>
       <c r="G11">
-        <v>2.0618087830267945E-3</v>
+        <v>8.8025159127544939E-3</v>
       </c>
       <c r="H11">
-        <v>-1.6316119816999625E-3</v>
+        <v>-1.0435350534517135E-2</v>
       </c>
       <c r="I11">
-        <v>3.7872386698837496E-2</v>
+        <v>6.3549667420949807E-2</v>
       </c>
       <c r="J11">
-        <v>1.2956087926007387E-3</v>
+        <v>-1.8884763082885753E-3</v>
       </c>
       <c r="K11">
-        <v>-5.0724779235327084E-4</v>
+        <v>9.939072593046435E-5</v>
       </c>
       <c r="L11">
-        <v>0.32546013979253258</v>
+        <v>0.40071703933056074</v>
       </c>
       <c r="M11">
-        <v>0.13822905109360953</v>
+        <v>0.1891061642012529</v>
       </c>
       <c r="N11">
-        <v>0.13877751525069174</v>
+        <v>0.18927396685125364</v>
       </c>
       <c r="O11">
-        <v>0.14094288062056839</v>
+        <v>0.19201225703033936</v>
       </c>
       <c r="P11">
-        <v>0.13642524629259536</v>
+        <v>0.18690227805592691</v>
       </c>
       <c r="Q11">
-        <v>0.13785851985849451</v>
+        <v>0.18776297744623732</v>
       </c>
       <c r="R11">
-        <v>0.13952857491760662</v>
+        <v>0.19080537975914158</v>
       </c>
       <c r="S11">
-        <v>0.13961045589861248</v>
+        <v>0.19073318105157361</v>
       </c>
       <c r="T11">
-        <v>0.13788649388700666</v>
+        <v>0.18962159228676551</v>
       </c>
       <c r="U11">
-        <v>0.14261457446171158</v>
+        <v>0.19408478138086677</v>
       </c>
       <c r="V11">
-        <v>0.13833042090879705</v>
+        <v>0.19010985351486348</v>
       </c>
       <c r="W11">
-        <v>-3.7503386531868715E-2</v>
+        <v>7.0786223483476102E-2</v>
       </c>
       <c r="X11">
-        <v>-5.9653397388223939E-4</v>
+        <v>-3.5332025381847299E-3</v>
       </c>
       <c r="Y11">
-        <v>-8.7450093713317981E-2</v>
+        <v>-0.19332056057601318</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -4441,76 +4442,76 @@
         <v>88</v>
       </c>
       <c r="B12" s="28">
-        <v>-3.3846715499224918E-2</v>
+        <v>0.2797295608539539</v>
       </c>
       <c r="C12">
-        <v>4.5163068018624162E-3</v>
+        <v>6.9220679436423418E-3</v>
       </c>
       <c r="D12">
-        <v>-1.0930141029429716E-2</v>
+        <v>-1.0904699692027738E-2</v>
       </c>
       <c r="E12">
-        <v>-1.9273324511565292E-3</v>
+        <v>4.0110970870882411E-3</v>
       </c>
       <c r="F12">
-        <v>-2.2954173392850073E-3</v>
+        <v>-4.5815373878275341E-3</v>
       </c>
       <c r="G12">
-        <v>1.1507578069408494E-2</v>
+        <v>1.495913678547614E-2</v>
       </c>
       <c r="H12">
-        <v>-1.3148131155760676E-3</v>
+        <v>-8.6671329194928717E-3</v>
       </c>
       <c r="I12">
-        <v>1.1919966010008595E-2</v>
+        <v>2.6150067191342219E-2</v>
       </c>
       <c r="J12">
-        <v>1.9824519917849264E-3</v>
+        <v>9.6499460693572417E-4</v>
       </c>
       <c r="K12">
-        <v>-4.7866177210160966E-5</v>
+        <v>8.3501032164255592E-5</v>
       </c>
       <c r="L12">
-        <v>0.13822905109360953</v>
+        <v>0.1891061642012529</v>
       </c>
       <c r="M12">
-        <v>0.22814298501401281</v>
+        <v>0.30409749386566765</v>
       </c>
       <c r="N12">
-        <v>0.13703868049445736</v>
+        <v>0.18703211373470402</v>
       </c>
       <c r="O12">
-        <v>0.13928066022962149</v>
+        <v>0.19048341310705832</v>
       </c>
       <c r="P12">
-        <v>0.13547065851406515</v>
+        <v>0.18555552805839842</v>
       </c>
       <c r="Q12">
-        <v>0.1369075191779808</v>
+        <v>0.1869722229027129</v>
       </c>
       <c r="R12">
-        <v>0.13884507419325101</v>
+        <v>0.18962668184200676</v>
       </c>
       <c r="S12">
-        <v>0.13827271145221542</v>
+        <v>0.18929820658552521</v>
       </c>
       <c r="T12">
-        <v>0.13729894599220865</v>
+        <v>0.18730787262394169</v>
       </c>
       <c r="U12">
-        <v>0.13976709720897484</v>
+        <v>0.19027875301512884</v>
       </c>
       <c r="V12">
-        <v>0.13888971722945245</v>
+        <v>0.18985528984816238</v>
       </c>
       <c r="W12">
-        <v>-0.47629053572111707</v>
+        <v>-0.72606337747770833</v>
       </c>
       <c r="X12">
-        <v>1.127844940061358E-2</v>
+        <v>1.5715366747501732E-2</v>
       </c>
       <c r="Y12">
-        <v>0.16870606570262309</v>
+        <v>0.30241143864756126</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -4518,76 +4519,76 @@
         <v>89</v>
       </c>
       <c r="B13" s="28">
-        <v>0.39730609805790379</v>
+        <v>0.73381773060193223</v>
       </c>
       <c r="C13">
-        <v>1.036561008173428E-2</v>
+        <v>1.7451689890816746E-2</v>
       </c>
       <c r="D13">
-        <v>-8.1863878695853168E-3</v>
+        <v>-8.937408573629943E-3</v>
       </c>
       <c r="E13">
-        <v>1.73419599372171E-3</v>
+        <v>5.0878896610192341E-3</v>
       </c>
       <c r="F13">
-        <v>-6.6196711599207803E-3</v>
+        <v>-1.1717316561958518E-2</v>
       </c>
       <c r="G13">
-        <v>3.8319754585348503E-3</v>
+        <v>6.0664421063431201E-3</v>
       </c>
       <c r="H13">
-        <v>-2.8539887751991705E-4</v>
+        <v>-5.2898114164224297E-3</v>
       </c>
       <c r="I13">
-        <v>-2.6637954924914609E-3</v>
+        <v>6.7453252365120953E-2</v>
       </c>
       <c r="J13">
-        <v>-3.0333166376464091E-4</v>
+        <v>-1.7803044128895246E-3</v>
       </c>
       <c r="K13">
-        <v>2.7249314730435053E-4</v>
+        <v>8.8745004312389521E-5</v>
       </c>
       <c r="L13">
-        <v>0.13877751525069174</v>
+        <v>0.18927396685125364</v>
       </c>
       <c r="M13">
-        <v>0.13703868049445736</v>
+        <v>0.18703211373470402</v>
       </c>
       <c r="N13">
-        <v>0.2547766222253004</v>
+        <v>0.33279185812201334</v>
       </c>
       <c r="O13">
-        <v>0.1385266821729628</v>
+        <v>0.19105742845284895</v>
       </c>
       <c r="P13">
-        <v>0.13549594227647477</v>
+        <v>0.18668192997179056</v>
       </c>
       <c r="Q13">
-        <v>0.13704354491561083</v>
+        <v>0.18681883557334117</v>
       </c>
       <c r="R13">
-        <v>0.13835143647315257</v>
+        <v>0.18975200989035329</v>
       </c>
       <c r="S13">
-        <v>0.13905906835222076</v>
+        <v>0.19042554188087848</v>
       </c>
       <c r="T13">
-        <v>0.13714168558349824</v>
+        <v>0.18951486497810319</v>
       </c>
       <c r="U13">
-        <v>0.14114969872977745</v>
+        <v>0.19378022843078829</v>
       </c>
       <c r="V13">
-        <v>0.13647566974159259</v>
+        <v>0.18913824308930896</v>
       </c>
       <c r="W13">
-        <v>0.11599415316129086</v>
+        <v>-3.8463226074749723E-3</v>
       </c>
       <c r="X13">
-        <v>-2.6961462379318088E-3</v>
+        <v>1.9541752136296997E-4</v>
       </c>
       <c r="Y13">
-        <v>-0.20870654950559547</v>
+        <v>-0.17521584172208476</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -4595,76 +4596,76 @@
         <v>90</v>
       </c>
       <c r="B14" s="28">
-        <v>-0.13781991042411104</v>
+        <v>0.2867535644992058</v>
       </c>
       <c r="C14">
-        <v>8.270172876976678E-3</v>
+        <v>1.4440825791191339E-2</v>
       </c>
       <c r="D14">
-        <v>-1.6046243935155365E-2</v>
+        <v>-1.4597769225485474E-2</v>
       </c>
       <c r="E14">
-        <v>-3.3167244440372723E-3</v>
+        <v>5.2441726494273158E-3</v>
       </c>
       <c r="F14">
-        <v>-5.9571927191093207E-3</v>
+        <v>-1.6600383072309089E-2</v>
       </c>
       <c r="G14">
-        <v>7.5495253552309571E-3</v>
+        <v>1.6070337363201723E-2</v>
       </c>
       <c r="H14">
-        <v>1.1583515079843926E-3</v>
+        <v>-2.2404681610428967E-3</v>
       </c>
       <c r="I14">
-        <v>3.9275171997395331E-2</v>
+        <v>6.2961990483366981E-2</v>
       </c>
       <c r="J14">
-        <v>1.0888739948411164E-3</v>
+        <v>2.2445298234975639E-3</v>
       </c>
       <c r="K14">
-        <v>-1.0779516239298311E-4</v>
+        <v>6.9153602464497297E-5</v>
       </c>
       <c r="L14">
-        <v>0.14094288062056839</v>
+        <v>0.19201225703033936</v>
       </c>
       <c r="M14">
-        <v>0.13928066022962149</v>
+        <v>0.19048341310705832</v>
       </c>
       <c r="N14">
-        <v>0.1385266821729628</v>
+        <v>0.19105742845284895</v>
       </c>
       <c r="O14">
-        <v>0.26155900867685528</v>
+        <v>0.36165162451999261</v>
       </c>
       <c r="P14">
-        <v>0.13691225119399403</v>
+        <v>0.18890838919191932</v>
       </c>
       <c r="Q14">
-        <v>0.1385482042308436</v>
+        <v>0.1895765035698575</v>
       </c>
       <c r="R14">
-        <v>0.14042672140561174</v>
+        <v>0.19360537668002203</v>
       </c>
       <c r="S14">
-        <v>0.14056313354411173</v>
+        <v>0.19374826294765113</v>
       </c>
       <c r="T14">
-        <v>0.13872615122187681</v>
+        <v>0.19148534418381091</v>
       </c>
       <c r="U14">
-        <v>0.14267622226087329</v>
+        <v>0.19500797028035471</v>
       </c>
       <c r="V14">
-        <v>0.13893919841289901</v>
+        <v>0.19102095956629414</v>
       </c>
       <c r="W14">
-        <v>-0.42615256513551447</v>
+        <v>-0.72233406193415584</v>
       </c>
       <c r="X14">
-        <v>9.8289830290368783E-3</v>
+        <v>1.6125037368900481E-2</v>
       </c>
       <c r="Y14">
-        <v>0.14522530054084687</v>
+        <v>0.29295095846103436</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -4672,76 +4673,76 @@
         <v>91</v>
       </c>
       <c r="B15" s="28">
-        <v>0.16923685457527518</v>
+        <v>0.38409203980643469</v>
       </c>
       <c r="C15">
-        <v>3.6326346137162159E-3</v>
+        <v>5.6513204836884101E-3</v>
       </c>
       <c r="D15">
-        <v>-2.8788524312352917E-3</v>
+        <v>-5.6020297237818761E-4</v>
       </c>
       <c r="E15">
-        <v>1.7582866181414109E-4</v>
+        <v>6.0858907004433943E-3</v>
       </c>
       <c r="F15">
-        <v>2.9973889028888333E-4</v>
+        <v>-1.1956730471953461E-2</v>
       </c>
       <c r="G15">
-        <v>2.1976760475354851E-3</v>
+        <v>1.0705885560449435E-2</v>
       </c>
       <c r="H15">
-        <v>2.4397538701321914E-3</v>
+        <v>-2.8561636157380249E-3</v>
       </c>
       <c r="I15">
-        <v>4.0937706280476521E-2</v>
+        <v>7.0303442078546108E-2</v>
       </c>
       <c r="J15">
-        <v>-4.5297912090492068E-4</v>
+        <v>-1.3761566682159027E-3</v>
       </c>
       <c r="K15">
-        <v>-1.0186499461616767E-3</v>
+        <v>1.0561772035569227E-4</v>
       </c>
       <c r="L15">
-        <v>0.13642524629259536</v>
+        <v>0.18690227805592691</v>
       </c>
       <c r="M15">
-        <v>0.13547065851406515</v>
+        <v>0.18555552805839842</v>
       </c>
       <c r="N15">
-        <v>0.13549594227647477</v>
+        <v>0.18668192997179056</v>
       </c>
       <c r="O15">
-        <v>0.13691225119399403</v>
+        <v>0.18890838919191932</v>
       </c>
       <c r="P15">
-        <v>0.2450004729428375</v>
+        <v>0.32667008326638342</v>
       </c>
       <c r="Q15">
-        <v>0.13604909093253664</v>
+        <v>0.18641514136237708</v>
       </c>
       <c r="R15">
-        <v>0.13647920357151694</v>
+        <v>0.18686687378306654</v>
       </c>
       <c r="S15">
-        <v>0.13700805709483871</v>
+        <v>0.18798826283785347</v>
       </c>
       <c r="T15">
-        <v>0.13557253126474933</v>
+        <v>0.18694342026590494</v>
       </c>
       <c r="U15">
-        <v>0.13804336856311111</v>
+        <v>0.18815583397774779</v>
       </c>
       <c r="V15">
-        <v>0.13505269994242194</v>
+        <v>0.18679119950985817</v>
       </c>
       <c r="W15">
-        <v>-0.11509244332893384</v>
+        <v>-0.60702832070221002</v>
       </c>
       <c r="X15">
-        <v>3.3610853237174112E-3</v>
+        <v>1.3925104862851095E-2</v>
       </c>
       <c r="Y15">
-        <v>-6.5207608733103981E-2</v>
+        <v>0.21857776684485214</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -4749,76 +4750,76 @@
         <v>92</v>
       </c>
       <c r="B16" s="28">
-        <v>-0.14049531099382473</v>
+        <v>0.42849320408399871</v>
       </c>
       <c r="C16">
-        <v>4.6511656485942153E-3</v>
+        <v>1.9766776784912593E-3</v>
       </c>
       <c r="D16">
-        <v>-8.2247944361459879E-3</v>
+        <v>-6.2085119454594606E-3</v>
       </c>
       <c r="E16">
-        <v>2.6732900577197682E-4</v>
+        <v>1.0366089694286873E-2</v>
       </c>
       <c r="F16">
-        <v>-7.9732776127569259E-3</v>
+        <v>-6.6405122162020956E-3</v>
       </c>
       <c r="G16">
-        <v>8.0673847068077967E-3</v>
+        <v>1.7384254433432625E-2</v>
       </c>
       <c r="H16">
-        <v>1.0944915455193931E-3</v>
+        <v>-1.531864003406741E-3</v>
       </c>
       <c r="I16">
-        <v>4.2429339555317164E-2</v>
+        <v>5.3631581734316036E-2</v>
       </c>
       <c r="J16">
-        <v>1.4143056169158182E-3</v>
+        <v>2.2121249963394374E-4</v>
       </c>
       <c r="K16">
-        <v>8.6987516164464644E-5</v>
+        <v>1.2934305696620874E-4</v>
       </c>
       <c r="L16">
-        <v>0.13785851985849451</v>
+        <v>0.18776297744623732</v>
       </c>
       <c r="M16">
-        <v>0.1369075191779808</v>
+        <v>0.1869722229027129</v>
       </c>
       <c r="N16">
-        <v>0.13704354491561083</v>
+        <v>0.18681883557334117</v>
       </c>
       <c r="O16">
-        <v>0.1385482042308436</v>
+        <v>0.1895765035698575</v>
       </c>
       <c r="P16">
-        <v>0.13604909093253664</v>
+        <v>0.18641514136237708</v>
       </c>
       <c r="Q16">
-        <v>0.22728092440897288</v>
+        <v>0.29391504697790449</v>
       </c>
       <c r="R16">
-        <v>0.13872974830375762</v>
+        <v>0.18993363646523581</v>
       </c>
       <c r="S16">
-        <v>0.13838720315095043</v>
+        <v>0.18979718142853658</v>
       </c>
       <c r="T16">
-        <v>0.13655551316437087</v>
+        <v>0.1874719901067915</v>
       </c>
       <c r="U16">
-        <v>0.13856897922970421</v>
+        <v>0.18877084444502645</v>
       </c>
       <c r="V16">
-        <v>0.13636254026823591</v>
+        <v>0.18791263205542014</v>
       </c>
       <c r="W16">
-        <v>6.5764027832735036E-2</v>
+        <v>-8.2335548991857022E-3</v>
       </c>
       <c r="X16">
-        <v>-1.6946303186395916E-3</v>
+        <v>-2.0717033716601083E-4</v>
       </c>
       <c r="Y16">
-        <v>-0.17588469911021309</v>
+        <v>-0.17635087517557402</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -4826,76 +4827,76 @@
         <v>93</v>
       </c>
       <c r="B17" s="28">
-        <v>-0.22188335905556267</v>
+        <v>-4.0235902478336694E-2</v>
       </c>
       <c r="C17">
-        <v>3.9272257873377067E-3</v>
+        <v>4.6846492494128228E-3</v>
       </c>
       <c r="D17">
-        <v>-1.2361470457209763E-2</v>
+        <v>-1.6382424858995062E-2</v>
       </c>
       <c r="E17">
-        <v>8.5844585569955917E-4</v>
+        <v>5.2912155902574247E-3</v>
       </c>
       <c r="F17">
-        <v>-1.0658843709390076E-2</v>
+        <v>-7.9437022184900979E-3</v>
       </c>
       <c r="G17">
-        <v>2.6863390895296373E-2</v>
+        <v>3.8423704110529359E-2</v>
       </c>
       <c r="H17">
-        <v>2.4723807910925419E-3</v>
+        <v>-2.4729128864216798E-3</v>
       </c>
       <c r="I17">
-        <v>3.9718345080824641E-2</v>
+        <v>6.4125504081869567E-2</v>
       </c>
       <c r="J17">
-        <v>3.354013412493825E-3</v>
+        <v>2.8940153707164608E-3</v>
       </c>
       <c r="K17">
-        <v>4.6777039952655523E-4</v>
+        <v>1.8961697431795946E-5</v>
       </c>
       <c r="L17">
-        <v>0.13952857491760662</v>
+        <v>0.19080537975914158</v>
       </c>
       <c r="M17">
-        <v>0.13884507419325101</v>
+        <v>0.18962668184200676</v>
       </c>
       <c r="N17">
-        <v>0.13835143647315257</v>
+        <v>0.18975200989035329</v>
       </c>
       <c r="O17">
-        <v>0.14042672140561174</v>
+        <v>0.19360537668002203</v>
       </c>
       <c r="P17">
-        <v>0.13647920357151694</v>
+        <v>0.18686687378306654</v>
       </c>
       <c r="Q17">
-        <v>0.13872974830375762</v>
+        <v>0.18993363646523581</v>
       </c>
       <c r="R17">
-        <v>0.21114807163570892</v>
+        <v>0.28225608280083775</v>
       </c>
       <c r="S17">
-        <v>0.14091502804559528</v>
+        <v>0.19411522269911713</v>
       </c>
       <c r="T17">
-        <v>0.13844860634705738</v>
+        <v>0.19029165437604778</v>
       </c>
       <c r="U17">
-        <v>0.14072479685219674</v>
+        <v>0.19365518163494377</v>
       </c>
       <c r="V17">
-        <v>0.13805389812207758</v>
+        <v>0.1901526002252997</v>
       </c>
       <c r="W17">
-        <v>5.7515752855614943E-2</v>
+        <v>9.7789982217011684E-2</v>
       </c>
       <c r="X17">
-        <v>-1.8835040584636656E-3</v>
+        <v>-3.8038996083055695E-3</v>
       </c>
       <c r="Y17">
-        <v>-0.17243155637274582</v>
+        <v>-0.23360105990890823</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -4903,76 +4904,76 @@
         <v>94</v>
       </c>
       <c r="B18" s="28">
-        <v>-0.24808631643640941</v>
+        <v>9.5244657500010946E-2</v>
       </c>
       <c r="C18">
-        <v>9.0164703008346822E-3</v>
+        <v>1.2686614753749284E-2</v>
       </c>
       <c r="D18">
-        <v>-1.136685627626529E-2</v>
+        <v>-1.1485756972139591E-2</v>
       </c>
       <c r="E18">
-        <v>-1.4058153812108454E-3</v>
+        <v>5.5514772783760852E-3</v>
       </c>
       <c r="F18">
-        <v>-9.3217748714856039E-3</v>
+        <v>-1.1219747640836412E-2</v>
       </c>
       <c r="G18">
-        <v>2.1122285969539918E-2</v>
+        <v>3.2754378936420261E-2</v>
       </c>
       <c r="H18">
-        <v>2.218659369730442E-3</v>
+        <v>9.2166909737528835E-4</v>
       </c>
       <c r="I18">
-        <v>4.1173819527528743E-2</v>
+        <v>6.8856750884901341E-2</v>
       </c>
       <c r="J18">
-        <v>1.1557299792795024E-3</v>
+        <v>1.9301016037318944E-3</v>
       </c>
       <c r="K18">
-        <v>2.8249183400097175E-4</v>
+        <v>8.1360577123522007E-5</v>
       </c>
       <c r="L18">
-        <v>0.13961045589861248</v>
+        <v>0.19073318105157361</v>
       </c>
       <c r="M18">
-        <v>0.13827271145221542</v>
+        <v>0.18929820658552521</v>
       </c>
       <c r="N18">
-        <v>0.13905906835222076</v>
+        <v>0.19042554188087848</v>
       </c>
       <c r="O18">
-        <v>0.14056313354411173</v>
+        <v>0.19374826294765113</v>
       </c>
       <c r="P18">
-        <v>0.13700805709483871</v>
+        <v>0.18798826283785347</v>
       </c>
       <c r="Q18">
-        <v>0.13838720315095043</v>
+        <v>0.18979718142853658</v>
       </c>
       <c r="R18">
-        <v>0.14091502804559528</v>
+        <v>0.19411522269911713</v>
       </c>
       <c r="S18">
-        <v>0.23041000744837092</v>
+        <v>0.31453233268032837</v>
       </c>
       <c r="T18">
-        <v>0.13859671052132089</v>
+        <v>0.19152767443232441</v>
       </c>
       <c r="U18">
-        <v>0.14205117081678353</v>
+        <v>0.19422897558934643</v>
       </c>
       <c r="V18">
-        <v>0.13806272961039726</v>
+        <v>0.18991762436398457</v>
       </c>
       <c r="W18">
-        <v>0.4847821570226748</v>
+        <v>0.66779087699612016</v>
       </c>
       <c r="X18">
-        <v>-1.0843384197784573E-2</v>
+        <v>-1.5832638096922175E-2</v>
       </c>
       <c r="Y18">
-        <v>-0.45761475908321869</v>
+        <v>-0.62132320106729944</v>
       </c>
     </row>
     <row r="19" spans="1:25">
@@ -4980,76 +4981,76 @@
         <v>95</v>
       </c>
       <c r="B19" s="28">
-        <v>-0.2496338898015889</v>
+        <v>0.34709555193946529</v>
       </c>
       <c r="C19">
-        <v>4.677629974442446E-3</v>
+        <v>1.0761750685467711E-2</v>
       </c>
       <c r="D19">
-        <v>-1.4576270915288583E-2</v>
+        <v>-1.7701984247219638E-2</v>
       </c>
       <c r="E19">
-        <v>-7.890926965583106E-3</v>
+        <v>-4.6745526778994434E-3</v>
       </c>
       <c r="F19">
-        <v>-6.3383861452735828E-3</v>
+        <v>-9.9687609496605708E-3</v>
       </c>
       <c r="G19">
-        <v>1.1381805881844204E-2</v>
+        <v>2.6220920390710695E-2</v>
       </c>
       <c r="H19">
-        <v>5.0724609843613572E-3</v>
+        <v>2.5447735050496134E-4</v>
       </c>
       <c r="I19">
-        <v>1.9657391728534201E-2</v>
+        <v>2.7564447175786766E-2</v>
       </c>
       <c r="J19">
-        <v>9.1289437508450255E-4</v>
+        <v>-1.1267893663378242E-3</v>
       </c>
       <c r="K19">
-        <v>5.768544494111922E-4</v>
+        <v>8.6534115583630241E-5</v>
       </c>
       <c r="L19">
-        <v>0.13788649388700666</v>
+        <v>0.18962159228676551</v>
       </c>
       <c r="M19">
-        <v>0.13729894599220865</v>
+        <v>0.18730787262394169</v>
       </c>
       <c r="N19">
-        <v>0.13714168558349824</v>
+        <v>0.18951486497810319</v>
       </c>
       <c r="O19">
-        <v>0.13872615122187681</v>
+        <v>0.19148534418381091</v>
       </c>
       <c r="P19">
-        <v>0.13557253126474933</v>
+        <v>0.18694342026590494</v>
       </c>
       <c r="Q19">
-        <v>0.13655551316437087</v>
+        <v>0.1874719901067915</v>
       </c>
       <c r="R19">
-        <v>0.13844860634705738</v>
+        <v>0.19029165437604778</v>
       </c>
       <c r="S19">
-        <v>0.13859671052132089</v>
+        <v>0.19152767443232441</v>
       </c>
       <c r="T19">
-        <v>0.33195554264354493</v>
+        <v>0.47243144039235108</v>
       </c>
       <c r="U19">
-        <v>0.14043637006728496</v>
+        <v>0.19447906190870481</v>
       </c>
       <c r="V19">
-        <v>0.13798798732221448</v>
+        <v>0.19023273428014406</v>
       </c>
       <c r="W19">
-        <v>0.1049260683066425</v>
+        <v>-4.1617124731729682E-2</v>
       </c>
       <c r="X19">
-        <v>-1.716221360690487E-3</v>
+        <v>1.7547418374308104E-3</v>
       </c>
       <c r="Y19">
-        <v>-0.21164515906158132</v>
+        <v>-0.15836539069987138</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -5057,76 +5058,76 @@
         <v>96</v>
       </c>
       <c r="B20" s="28">
-        <v>-0.23703830407842028</v>
+        <v>1.3450726515789881E-2</v>
       </c>
       <c r="C20">
-        <v>1.7802789660290051E-2</v>
+        <v>3.0078683257696727E-2</v>
       </c>
       <c r="D20">
-        <v>-2.0700040476634624E-2</v>
+        <v>-2.5915912104090617E-2</v>
       </c>
       <c r="E20">
-        <v>-9.9409563042813995E-3</v>
+        <v>-8.8346045426468747E-3</v>
       </c>
       <c r="F20">
-        <v>-2.7404599490629573E-3</v>
+        <v>-8.4462357562314939E-3</v>
       </c>
       <c r="G20">
-        <v>1.4355189390636861E-2</v>
+        <v>2.3804769729267136E-2</v>
       </c>
       <c r="H20">
-        <v>6.3329104904553297E-3</v>
+        <v>5.1830568021328516E-3</v>
       </c>
       <c r="I20">
-        <v>4.3251802117939608E-2</v>
+        <v>6.9694960238182668E-2</v>
       </c>
       <c r="J20">
-        <v>-1.2741078469166167E-3</v>
+        <v>-2.8450322456401028E-3</v>
       </c>
       <c r="K20">
-        <v>-3.3581427123569908E-4</v>
+        <v>-1.9968931484756918E-5</v>
       </c>
       <c r="L20">
-        <v>0.14261457446171158</v>
+        <v>0.19408478138086677</v>
       </c>
       <c r="M20">
-        <v>0.13976709720897484</v>
+        <v>0.19027875301512884</v>
       </c>
       <c r="N20">
-        <v>0.14114969872977745</v>
+        <v>0.19378022843078829</v>
       </c>
       <c r="O20">
-        <v>0.14267622226087329</v>
+        <v>0.19500797028035471</v>
       </c>
       <c r="P20">
-        <v>0.13804336856311111</v>
+        <v>0.18815583397774779</v>
       </c>
       <c r="Q20">
-        <v>0.13856897922970421</v>
+        <v>0.18877084444502645</v>
       </c>
       <c r="R20">
-        <v>0.14072479685219674</v>
+        <v>0.19365518163494377</v>
       </c>
       <c r="S20">
-        <v>0.14205117081678353</v>
+        <v>0.19422897558934643</v>
       </c>
       <c r="T20">
-        <v>0.14043637006728496</v>
+        <v>0.19447906190870481</v>
       </c>
       <c r="U20">
-        <v>0.29594824973281159</v>
+        <v>0.39266768298086474</v>
       </c>
       <c r="V20">
-        <v>0.13869640789632268</v>
+        <v>0.19090255234737857</v>
       </c>
       <c r="W20">
-        <v>0.21760313856555041</v>
+        <v>0.22346771741558402</v>
       </c>
       <c r="X20">
-        <v>-5.4010660469046672E-3</v>
+        <v>-6.7519442816171248E-3</v>
       </c>
       <c r="Y20">
-        <v>-0.26433693905838362</v>
+        <v>-0.29443021758590893</v>
       </c>
     </row>
     <row r="21" spans="1:25">
@@ -5134,76 +5135,76 @@
         <v>97</v>
       </c>
       <c r="B21" s="28">
-        <v>-0.37214961042727246</v>
+        <v>0.19891318272947825</v>
       </c>
       <c r="C21">
-        <v>6.3206753664585905E-3</v>
+        <v>9.23838811834507E-3</v>
       </c>
       <c r="D21">
-        <v>-1.1480691743811389E-2</v>
+        <v>-1.2049797758661496E-2</v>
       </c>
       <c r="E21">
-        <v>-7.4874865499970356E-3</v>
+        <v>3.2369187177399145E-3</v>
       </c>
       <c r="F21">
-        <v>-6.8614152929517072E-3</v>
+        <v>2.3106493170582665E-5</v>
       </c>
       <c r="G21">
-        <v>6.2169779290617289E-3</v>
+        <v>1.2762979654432599E-2</v>
       </c>
       <c r="H21">
-        <v>-5.386090787335443E-3</v>
+        <v>-7.8847001118066973E-3</v>
       </c>
       <c r="I21">
-        <v>3.7901231694003723E-2</v>
+        <v>6.8159608276641359E-2</v>
       </c>
       <c r="J21">
-        <v>1.5356764501257836E-3</v>
+        <v>-1.2180361960801023E-3</v>
       </c>
       <c r="K21">
-        <v>6.4430694030079803E-4</v>
+        <v>1.5171193759525069E-4</v>
       </c>
       <c r="L21">
-        <v>0.13833042090879705</v>
+        <v>0.19010985351486348</v>
       </c>
       <c r="M21">
-        <v>0.13888971722945245</v>
+        <v>0.18985528984816238</v>
       </c>
       <c r="N21">
-        <v>0.13647566974159259</v>
+        <v>0.18913824308930896</v>
       </c>
       <c r="O21">
-        <v>0.13893919841289901</v>
+        <v>0.19102095956629414</v>
       </c>
       <c r="P21">
-        <v>0.13505269994242194</v>
+        <v>0.18679119950985817</v>
       </c>
       <c r="Q21">
-        <v>0.13636254026823591</v>
+        <v>0.18791263205542014</v>
       </c>
       <c r="R21">
-        <v>0.13805389812207758</v>
+        <v>0.1901526002252997</v>
       </c>
       <c r="S21">
-        <v>0.13806272961039726</v>
+        <v>0.18991762436398457</v>
       </c>
       <c r="T21">
-        <v>0.13798798732221448</v>
+        <v>0.19023273428014406</v>
       </c>
       <c r="U21">
-        <v>0.13869640789632268</v>
+        <v>0.19090255234737857</v>
       </c>
       <c r="V21">
-        <v>0.28520797104145335</v>
+        <v>0.42004500264454547</v>
       </c>
       <c r="W21">
-        <v>-0.48756932160776489</v>
+        <v>-0.63181997319708749</v>
       </c>
       <c r="X21">
-        <v>1.2286298802938333E-2</v>
+        <v>1.5853738601201622E-2</v>
       </c>
       <c r="Y21">
-        <v>0.16985752770684215</v>
+        <v>0.21094408675263757</v>
       </c>
     </row>
     <row r="22" spans="1:25">
@@ -5211,76 +5212,76 @@
         <v>145</v>
       </c>
       <c r="B22" s="28">
-        <v>42.179682434095078</v>
+        <v>50.145408985199175</v>
       </c>
       <c r="C22">
-        <v>-0.12859751300421518</v>
+        <v>-0.49909184781068894</v>
       </c>
       <c r="D22">
-        <v>0.1770734298214712</v>
+        <v>0.30259720862195666</v>
       </c>
       <c r="E22">
-        <v>6.2142406410686524E-3</v>
+        <v>0.17187058027941179</v>
       </c>
       <c r="F22">
-        <v>-9.4748967033658829E-3</v>
+        <v>-3.7449364467653252E-3</v>
       </c>
       <c r="G22">
-        <v>0.44835790866042852</v>
+        <v>0.67520338388582224</v>
       </c>
       <c r="H22">
-        <v>0.16581199600601518</v>
+        <v>0.19026725533048905</v>
       </c>
       <c r="I22">
-        <v>0.80297652089649851</v>
+        <v>1.243657955007619</v>
       </c>
       <c r="J22">
-        <v>9.732603082362172E-2</v>
+        <v>0.1487602517616321</v>
       </c>
       <c r="K22">
-        <v>4.3378494090640981E-3</v>
+        <v>-1.1724764118938046E-3</v>
       </c>
       <c r="L22">
-        <v>-3.7503386531868715E-2</v>
+        <v>7.0786223483476102E-2</v>
       </c>
       <c r="M22">
-        <v>-0.47629053572111707</v>
+        <v>-0.72606337747770833</v>
       </c>
       <c r="N22">
-        <v>0.11599415316129086</v>
+        <v>-3.8463226074749723E-3</v>
       </c>
       <c r="O22">
-        <v>-0.42615256513551447</v>
+        <v>-0.72233406193415584</v>
       </c>
       <c r="P22">
-        <v>-0.11509244332893384</v>
+        <v>-0.60702832070221002</v>
       </c>
       <c r="Q22">
-        <v>6.5764027832735036E-2</v>
+        <v>-8.2335548991857022E-3</v>
       </c>
       <c r="R22">
-        <v>5.7515752855614943E-2</v>
+        <v>9.7789982217011684E-2</v>
       </c>
       <c r="S22">
-        <v>0.4847821570226748</v>
+        <v>0.66779087699612016</v>
       </c>
       <c r="T22">
-        <v>0.1049260683066425</v>
+        <v>-4.1617124731729682E-2</v>
       </c>
       <c r="U22">
-        <v>0.21760313856555041</v>
+        <v>0.22346771741558402</v>
       </c>
       <c r="V22">
-        <v>-0.48756932160776489</v>
+        <v>-0.63181997319708749</v>
       </c>
       <c r="W22">
-        <v>552.37737274383687</v>
+        <v>697.40510602159395</v>
       </c>
       <c r="X22">
-        <v>-12.573855322478787</v>
+        <v>-15.883347604547385</v>
       </c>
       <c r="Y22">
-        <v>-363.25255138877515</v>
+        <v>-458.43589242199107</v>
       </c>
     </row>
     <row r="23" spans="1:25">
@@ -5288,76 +5289,76 @@
         <v>141</v>
       </c>
       <c r="B23" s="28">
-        <v>-1.011127669650139</v>
+        <v>-1.2169192910445317</v>
       </c>
       <c r="C23">
-        <v>1.2878847130870961E-3</v>
+        <v>9.4308232184674781E-3</v>
       </c>
       <c r="D23">
-        <v>-3.5638620644135198E-3</v>
+        <v>-5.8798245187188123E-3</v>
       </c>
       <c r="E23">
-        <v>6.7409750167927432E-4</v>
+        <v>-3.0855420892277148E-3</v>
       </c>
       <c r="F23">
-        <v>-4.3509181755516579E-4</v>
+        <v>-2.5863207909175687E-4</v>
       </c>
       <c r="G23">
-        <v>-9.0805752208120514E-3</v>
+        <v>-1.2753389154642867E-2</v>
       </c>
       <c r="H23">
-        <v>-3.7589510799761962E-3</v>
+        <v>-4.427860264708228E-3</v>
       </c>
       <c r="I23">
-        <v>-1.6209879001932173E-2</v>
+        <v>-2.4206046454630925E-2</v>
       </c>
       <c r="J23">
-        <v>-2.2591520193440697E-3</v>
+        <v>-3.5649193954222919E-3</v>
       </c>
       <c r="K23">
-        <v>-5.9376932972964031E-5</v>
+        <v>2.4345436624344039E-5</v>
       </c>
       <c r="L23">
-        <v>-5.9653397388223939E-4</v>
+        <v>-3.5332025381847299E-3</v>
       </c>
       <c r="M23">
-        <v>1.127844940061358E-2</v>
+        <v>1.5715366747501732E-2</v>
       </c>
       <c r="N23">
-        <v>-2.6961462379318088E-3</v>
+        <v>1.9541752136296997E-4</v>
       </c>
       <c r="O23">
-        <v>9.8289830290368783E-3</v>
+        <v>1.6125037368900481E-2</v>
       </c>
       <c r="P23">
-        <v>3.3610853237174112E-3</v>
+        <v>1.3925104862851095E-2</v>
       </c>
       <c r="Q23">
-        <v>-1.6946303186395916E-3</v>
+        <v>-2.0717033716601083E-4</v>
       </c>
       <c r="R23">
-        <v>-1.8835040584636656E-3</v>
+        <v>-3.8038996083055695E-3</v>
       </c>
       <c r="S23">
-        <v>-1.0843384197784573E-2</v>
+        <v>-1.5832638096922175E-2</v>
       </c>
       <c r="T23">
-        <v>-1.716221360690487E-3</v>
+        <v>1.7547418374308104E-3</v>
       </c>
       <c r="U23">
-        <v>-5.4010660469046672E-3</v>
+        <v>-6.7519442816171248E-3</v>
       </c>
       <c r="V23">
-        <v>1.2286298802938333E-2</v>
+        <v>1.5853738601201622E-2</v>
       </c>
       <c r="W23">
-        <v>-12.573855322478787</v>
+        <v>-15.883347604547385</v>
       </c>
       <c r="X23">
-        <v>0.28920828836471713</v>
+        <v>0.36558256194946082</v>
       </c>
       <c r="Y23">
-        <v>8.2279481890129098</v>
+        <v>10.38903520851577</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -5365,76 +5366,76 @@
         <v>29</v>
       </c>
       <c r="B24" s="28">
-        <v>-23.28697614320123</v>
+        <v>-28.366486641942963</v>
       </c>
       <c r="C24">
-        <v>0.10062466744780638</v>
+        <v>0.35850112933657174</v>
       </c>
       <c r="D24">
-        <v>-0.16574530152585606</v>
+        <v>-0.26976885796582967</v>
       </c>
       <c r="E24">
-        <v>-8.186503916477611E-2</v>
+        <v>-0.21544635656109054</v>
       </c>
       <c r="F24">
-        <v>6.1738594960714238E-3</v>
+        <v>-1.169781030315196E-2</v>
       </c>
       <c r="G24">
-        <v>-0.34254788914150153</v>
+        <v>-0.52783804092838593</v>
       </c>
       <c r="H24">
-        <v>-0.13297975441268098</v>
+        <v>-0.15299354988962166</v>
       </c>
       <c r="I24">
-        <v>-0.61752305240079197</v>
+        <v>-0.94747786620384689</v>
       </c>
       <c r="J24">
-        <v>-8.7895924857041868E-2</v>
+        <v>-0.1270444315462424</v>
       </c>
       <c r="K24">
-        <v>-4.3345736870255723E-3</v>
+        <v>3.3640744664203092E-4</v>
       </c>
       <c r="L24">
-        <v>-8.7450093713317981E-2</v>
+        <v>-0.19332056057601318</v>
       </c>
       <c r="M24">
-        <v>0.16870606570262309</v>
+        <v>0.30241143864756126</v>
       </c>
       <c r="N24">
-        <v>-0.20870654950559547</v>
+        <v>-0.17521584172208476</v>
       </c>
       <c r="O24">
-        <v>0.14522530054084687</v>
+        <v>0.29295095846103436</v>
       </c>
       <c r="P24">
-        <v>-6.5207608733103981E-2</v>
+        <v>0.21857776684485214</v>
       </c>
       <c r="Q24">
-        <v>-0.17588469911021309</v>
+        <v>-0.17635087517557402</v>
       </c>
       <c r="R24">
-        <v>-0.17243155637274582</v>
+        <v>-0.23360105990890823</v>
       </c>
       <c r="S24">
-        <v>-0.45761475908321869</v>
+        <v>-0.62132320106729944</v>
       </c>
       <c r="T24">
-        <v>-0.21164515906158132</v>
+        <v>-0.15836539069987138</v>
       </c>
       <c r="U24">
-        <v>-0.26433693905838362</v>
+        <v>-0.29443021758590893</v>
       </c>
       <c r="V24">
-        <v>0.16985752770684215</v>
+        <v>0.21094408675263757</v>
       </c>
       <c r="W24">
-        <v>-363.25255138877515</v>
+        <v>-458.43589242199107</v>
       </c>
       <c r="X24">
-        <v>8.2279481890129098</v>
+        <v>10.38903520851577</v>
       </c>
       <c r="Y24">
-        <v>239.70960398760809</v>
+        <v>302.41363316006527</v>
       </c>
     </row>
   </sheetData>
@@ -5446,7 +5447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6790290-45A4-4DB4-B610-7B89AD61C200}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>

<commit_message>
Update estimates of I4b
</commit_message>
<xml_diff>
--- a/input/reg_income.xlsx
+++ b/input/reg_income.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD0F82A-DFD3-44F6-8B77-2882BA0C24A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99652F54-62AF-4485-A5D9-D21C10B1DE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" tabRatio="852" firstSheet="9" activeTab="15" xr2:uid="{8DDB884B-4CBA-4D96-8159-4841B9678181}"/>
+    <workbookView xWindow="870" yWindow="990" windowWidth="21480" windowHeight="18825" tabRatio="852" firstSheet="9" activeTab="11" xr2:uid="{8DDB884B-4CBA-4D96-8159-4841B9678181}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="7" r:id="rId1"/>
@@ -5454,7 +5454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6790290-45A4-4DB4-B610-7B89AD61C200}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5533,7 +5533,7 @@
         <v>97</v>
       </c>
       <c r="X1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="Y1" t="s">
         <v>141</v>
@@ -5547,79 +5547,79 @@
         <v>83</v>
       </c>
       <c r="B2" s="28">
-        <v>-0.23244205621507016</v>
+        <v>-0.20475170555878522</v>
       </c>
       <c r="C2">
-        <v>8.3636584051049144E-4</v>
+        <v>3.8954521771447821E-4</v>
       </c>
       <c r="D2">
-        <v>-5.4669207550457806E-6</v>
+        <v>-2.5728771529970379E-6</v>
       </c>
       <c r="E2">
-        <v>3.8645236738103425E-5</v>
+        <v>4.2898498299615093E-5</v>
       </c>
       <c r="F2">
-        <v>6.0988703076410994E-5</v>
+        <v>5.4809003903031825E-5</v>
       </c>
       <c r="G2">
-        <v>9.9074810380162318E-4</v>
+        <v>5.3136151070727351E-4</v>
       </c>
       <c r="H2">
-        <v>8.8605321813985463E-5</v>
+        <v>1.5719330222309109E-5</v>
       </c>
       <c r="I2">
-        <v>3.7567933403402295E-4</v>
+        <v>1.0424941899692119E-4</v>
       </c>
       <c r="J2">
-        <v>-3.2245710373524409E-5</v>
+        <v>-8.6716598173288383E-6</v>
       </c>
       <c r="K2">
-        <v>6.1180726592585557E-5</v>
+        <v>3.5403752053530006E-5</v>
       </c>
       <c r="L2">
-        <v>-2.2895840303450293E-5</v>
+        <v>-2.2090367625242965E-5</v>
       </c>
       <c r="M2">
-        <v>-9.4592243848465947E-5</v>
+        <v>-1.930560705739031E-5</v>
       </c>
       <c r="N2">
-        <v>-6.8346612950282923E-5</v>
+        <v>2.0776557835880914E-5</v>
       </c>
       <c r="O2">
-        <v>-2.6691493729107639E-5</v>
+        <v>-1.2147216036976181E-6</v>
       </c>
       <c r="P2">
-        <v>5.9759702456547732E-5</v>
+        <v>4.2734456843327058E-5</v>
       </c>
       <c r="Q2">
-        <v>-3.2262003646115118E-6</v>
+        <v>1.0399314842201701E-5</v>
       </c>
       <c r="R2">
-        <v>-6.5930193543487729E-5</v>
+        <v>2.0409188832499862E-5</v>
       </c>
       <c r="S2">
-        <v>-4.2587369656575495E-5</v>
+        <v>2.3163108354805687E-5</v>
       </c>
       <c r="T2">
-        <v>6.5819183852231129E-5</v>
+        <v>3.7923589918188554E-5</v>
       </c>
       <c r="U2">
-        <v>-9.1381558844600558E-5</v>
+        <v>-5.7459094906387592E-6</v>
       </c>
       <c r="V2">
-        <v>1.8962509263316385E-5</v>
+        <v>2.4339083856935242E-5</v>
       </c>
       <c r="W2">
-        <v>1.0291523765571312E-4</v>
+        <v>4.7464694847966157E-5</v>
       </c>
       <c r="X2">
-        <v>-2.3516350996442004E-3</v>
+        <v>-6.5626493354240673E-4</v>
       </c>
       <c r="Y2">
-        <v>4.3539395007997223E-5</v>
+        <v>-6.339269094192846E-6</v>
       </c>
       <c r="Z2">
-        <v>-3.0139394804159503E-2</v>
+        <v>-1.3954021316085516E-2</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -5627,79 +5627,79 @@
         <v>84</v>
       </c>
       <c r="B3" s="28">
-        <v>1.460651158390016E-3</v>
+        <v>1.2992100382615479E-3</v>
       </c>
       <c r="C3">
-        <v>-5.4669207550457806E-6</v>
+        <v>-2.5728771529970379E-6</v>
       </c>
       <c r="D3">
-        <v>3.5875115496883386E-8</v>
+        <v>1.7054575521191743E-8</v>
       </c>
       <c r="E3">
-        <v>-2.1368062572287876E-7</v>
+        <v>-2.6095899790955069E-7</v>
       </c>
       <c r="F3">
-        <v>-4.4028191089664755E-7</v>
+        <v>-3.7131540009833895E-7</v>
       </c>
       <c r="G3">
-        <v>-6.388396109980598E-6</v>
+        <v>-3.4717390237992772E-6</v>
       </c>
       <c r="H3">
-        <v>-6.6697943535855135E-7</v>
+        <v>-1.3431323760227534E-7</v>
       </c>
       <c r="I3">
-        <v>-2.3251328124177905E-6</v>
+        <v>-6.4626443055687164E-7</v>
       </c>
       <c r="J3">
-        <v>2.1364090698061375E-7</v>
+        <v>6.0800442814289225E-8</v>
       </c>
       <c r="K3">
-        <v>-3.685521129824482E-7</v>
+        <v>-2.241420469668203E-7</v>
       </c>
       <c r="L3">
-        <v>1.2226728446275103E-7</v>
+        <v>1.3693892431078282E-7</v>
       </c>
       <c r="M3">
-        <v>5.7887817223021307E-7</v>
+        <v>1.0741127371869533E-7</v>
       </c>
       <c r="N3">
-        <v>3.9913128490829598E-7</v>
+        <v>-1.7018896511829257E-7</v>
       </c>
       <c r="O3">
-        <v>8.1953104917087177E-8</v>
+        <v>-3.6363855614194652E-8</v>
       </c>
       <c r="P3">
-        <v>-4.2092067576003186E-7</v>
+        <v>-3.1098703171011699E-7</v>
       </c>
       <c r="Q3">
-        <v>-5.3535383524400343E-9</v>
+        <v>-1.0083302118018867E-7</v>
       </c>
       <c r="R3">
-        <v>3.3827118408761908E-7</v>
+        <v>-1.8965834056824574E-7</v>
       </c>
       <c r="S3">
-        <v>2.0682632061465967E-7</v>
+        <v>-1.9136278392855455E-7</v>
       </c>
       <c r="T3">
-        <v>-5.1410633012882669E-7</v>
+        <v>-3.0076477070616167E-7</v>
       </c>
       <c r="U3">
-        <v>5.4238921900210324E-7</v>
+        <v>-3.139509319576299E-9</v>
       </c>
       <c r="V3">
-        <v>-1.4517630199039434E-7</v>
+        <v>-1.8219952600717935E-7</v>
       </c>
       <c r="W3">
-        <v>-6.8812246098283263E-7</v>
+        <v>-3.456040478281387E-7</v>
       </c>
       <c r="X3">
-        <v>1.3761519885148107E-5</v>
+        <v>4.8721450278470485E-6</v>
       </c>
       <c r="Y3">
-        <v>-2.4952345962033938E-7</v>
+        <v>3.5934411351696912E-8</v>
       </c>
       <c r="Z3">
-        <v>1.9735474045139059E-4</v>
+        <v>9.140888467813529E-5</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -5707,79 +5707,79 @@
         <v>99</v>
       </c>
       <c r="B4" s="28">
-        <v>-0.18065185253441596</v>
+        <v>-0.18397702253874751</v>
       </c>
       <c r="C4">
-        <v>3.8645236738103425E-5</v>
+        <v>4.2898498299615093E-5</v>
       </c>
       <c r="D4">
-        <v>-2.1368062572287876E-7</v>
+        <v>-2.6095899790955069E-7</v>
       </c>
       <c r="E4">
-        <v>1.3634827154148138E-3</v>
+        <v>7.8197989679842353E-4</v>
       </c>
       <c r="F4">
-        <v>1.0041926267817343E-3</v>
+        <v>6.5331933811645397E-4</v>
       </c>
       <c r="G4">
-        <v>6.4752960705499437E-4</v>
+        <v>5.8719503971889429E-4</v>
       </c>
       <c r="H4">
-        <v>2.976442973231429E-5</v>
+        <v>-5.683802682867253E-5</v>
       </c>
       <c r="I4">
-        <v>2.6728937961888449E-5</v>
+        <v>1.2962781811681138E-5</v>
       </c>
       <c r="J4">
-        <v>4.1148245902515316E-5</v>
+        <v>8.0411296576683364E-6</v>
       </c>
       <c r="K4">
-        <v>6.2870510822546805E-5</v>
+        <v>3.4631236955086304E-5</v>
       </c>
       <c r="L4">
-        <v>3.4335274356937589E-6</v>
+        <v>-6.2752627584818259E-6</v>
       </c>
       <c r="M4">
-        <v>-4.4831727718894259E-4</v>
+        <v>-1.8745124017001866E-4</v>
       </c>
       <c r="N4">
-        <v>-4.2339523174762133E-4</v>
+        <v>-1.876365310173739E-4</v>
       </c>
       <c r="O4">
-        <v>-2.5770843396612236E-4</v>
+        <v>-1.388882832725449E-4</v>
       </c>
       <c r="P4">
-        <v>-3.6790244928033345E-4</v>
+        <v>-1.6192015913526063E-4</v>
       </c>
       <c r="Q4">
-        <v>-3.051954617120086E-4</v>
+        <v>-1.5434046213837145E-4</v>
       </c>
       <c r="R4">
-        <v>-2.6714371800515171E-4</v>
+        <v>-1.3706720043480102E-4</v>
       </c>
       <c r="S4">
-        <v>-2.6152777635922767E-4</v>
+        <v>-1.2633399493739594E-4</v>
       </c>
       <c r="T4">
-        <v>-3.6172391422070857E-4</v>
+        <v>-1.2890844974696255E-4</v>
       </c>
       <c r="U4">
-        <v>-4.2923649245604599E-4</v>
+        <v>-1.7128649949495859E-4</v>
       </c>
       <c r="V4">
-        <v>-3.2635754230038108E-4</v>
+        <v>-1.3350623327530031E-4</v>
       </c>
       <c r="W4">
-        <v>-3.0472378371160604E-4</v>
+        <v>-1.1696938037380653E-4</v>
       </c>
       <c r="X4">
-        <v>3.1598423342782539E-3</v>
+        <v>1.3172606675703532E-3</v>
       </c>
       <c r="Y4">
-        <v>-5.7366322052473115E-5</v>
+        <v>-4.6210554317454249E-6</v>
       </c>
       <c r="Z4">
-        <v>-5.0962908247237926E-3</v>
+        <v>-3.590713747542564E-3</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -5787,79 +5787,79 @@
         <v>100</v>
       </c>
       <c r="B5" s="28">
-        <v>-0.27269281364085696</v>
+        <v>-0.29395302383329419</v>
       </c>
       <c r="C5">
-        <v>6.0988703076410994E-5</v>
+        <v>5.4809003903031825E-5</v>
       </c>
       <c r="D5">
-        <v>-4.4028191089664755E-7</v>
+        <v>-3.7131540009833895E-7</v>
       </c>
       <c r="E5">
-        <v>1.0041926267817343E-3</v>
+        <v>6.5331933811645397E-4</v>
       </c>
       <c r="F5">
-        <v>1.5522899163556143E-3</v>
+        <v>8.864479532081171E-4</v>
       </c>
       <c r="G5">
-        <v>5.8509130623549295E-4</v>
+        <v>4.710968787071266E-4</v>
       </c>
       <c r="H5">
-        <v>-1.5507832220929295E-5</v>
+        <v>-6.8083728076814297E-5</v>
       </c>
       <c r="I5">
-        <v>-3.4222339019402922E-5</v>
+        <v>-1.4966712754450667E-5</v>
       </c>
       <c r="J5">
-        <v>4.7397751599940414E-5</v>
+        <v>1.479434067412174E-5</v>
       </c>
       <c r="K5">
-        <v>8.6953927290429141E-5</v>
+        <v>4.7468083932424074E-5</v>
       </c>
       <c r="L5">
-        <v>1.6382202428623648E-5</v>
+        <v>7.6138695030735556E-7</v>
       </c>
       <c r="M5">
-        <v>-3.7610140768106387E-4</v>
+        <v>-1.070704165780817E-4</v>
       </c>
       <c r="N5">
-        <v>-3.7465494538696493E-4</v>
+        <v>-1.2776670766947616E-4</v>
       </c>
       <c r="O5">
-        <v>-3.1174040395174816E-4</v>
+        <v>-8.9296990456226902E-5</v>
       </c>
       <c r="P5">
-        <v>-3.7918439509132188E-4</v>
+        <v>-1.1659716042343161E-4</v>
       </c>
       <c r="Q5">
-        <v>-3.8023980269021436E-4</v>
+        <v>-1.4844482791552904E-4</v>
       </c>
       <c r="R5">
-        <v>-2.7823869007108717E-4</v>
+        <v>-1.0247255024790043E-4</v>
       </c>
       <c r="S5">
-        <v>-2.6774173849786588E-4</v>
+        <v>-8.5871971464446272E-5</v>
       </c>
       <c r="T5">
-        <v>-2.9718166205165047E-4</v>
+        <v>-6.9829062721032292E-5</v>
       </c>
       <c r="U5">
-        <v>-4.5650319825589405E-4</v>
+        <v>-1.2778979179038668E-4</v>
       </c>
       <c r="V5">
-        <v>-2.9998103400542082E-4</v>
+        <v>-8.7746162073782519E-5</v>
       </c>
       <c r="W5">
-        <v>-3.4162095096205753E-4</v>
+        <v>-8.2532978349576227E-5</v>
       </c>
       <c r="X5">
-        <v>1.6806629907650285E-2</v>
+        <v>1.2650437214488245E-3</v>
       </c>
       <c r="Y5">
-        <v>-3.9249377718462335E-4</v>
+        <v>2.0853709752339351E-7</v>
       </c>
       <c r="Z5">
-        <v>-1.4411966902579655E-2</v>
+        <v>-4.1013676924257798E-3</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -5867,79 +5867,79 @@
         <v>103</v>
       </c>
       <c r="B6" s="28">
-        <v>-2.1219240996627384E-3</v>
+        <v>8.6108629003347082E-3</v>
       </c>
       <c r="C6">
-        <v>9.9074810380162318E-4</v>
+        <v>5.3136151070727351E-4</v>
       </c>
       <c r="D6">
-        <v>-6.388396109980598E-6</v>
+        <v>-3.4717390237992772E-6</v>
       </c>
       <c r="E6">
-        <v>6.4752960705499437E-4</v>
+        <v>5.8719503971889429E-4</v>
       </c>
       <c r="F6">
-        <v>5.8509130623549295E-4</v>
+        <v>4.710968787071266E-4</v>
       </c>
       <c r="G6">
-        <v>2.7400770951757435E-2</v>
+        <v>3.883755338343263E-2</v>
       </c>
       <c r="H6">
-        <v>2.9434168276576411E-4</v>
+        <v>8.1688846746337876E-5</v>
       </c>
       <c r="I6">
-        <v>7.5782904484281849E-4</v>
+        <v>2.4447737503135135E-4</v>
       </c>
       <c r="J6">
-        <v>-1.235074849913667E-4</v>
+        <v>-3.3909078767468612E-5</v>
       </c>
       <c r="K6">
-        <v>8.8851347908823746E-7</v>
+        <v>-1.306939603770932E-4</v>
       </c>
       <c r="L6">
-        <v>1.173872549130716E-4</v>
+        <v>1.5446671979272284E-4</v>
       </c>
       <c r="M6">
-        <v>-4.2294873251084303E-4</v>
+        <v>-2.0300989717377416E-4</v>
       </c>
       <c r="N6">
-        <v>-5.219010744585092E-4</v>
+        <v>-1.6478838457802212E-4</v>
       </c>
       <c r="O6">
-        <v>-2.8911914461411171E-4</v>
+        <v>-9.2479255672741571E-5</v>
       </c>
       <c r="P6">
-        <v>-3.9753732376365597E-4</v>
+        <v>-1.3168394035841056E-4</v>
       </c>
       <c r="Q6">
-        <v>9.8221918369822985E-5</v>
+        <v>4.5569941411718624E-5</v>
       </c>
       <c r="R6">
-        <v>-2.6180768963694019E-4</v>
+        <v>-1.1988575043978423E-4</v>
       </c>
       <c r="S6">
-        <v>1.8355622887480591E-6</v>
+        <v>3.6849710356013157E-4</v>
       </c>
       <c r="T6">
-        <v>-7.875914842202323E-5</v>
+        <v>-6.9678050691199603E-6</v>
       </c>
       <c r="U6">
-        <v>-2.9133596961072438E-4</v>
+        <v>-4.8048469678683287E-5</v>
       </c>
       <c r="V6">
-        <v>-3.265505256146873E-4</v>
+        <v>-1.3279619219293704E-4</v>
       </c>
       <c r="W6">
-        <v>-2.9387536816245438E-4</v>
+        <v>-1.7427317757796705E-4</v>
       </c>
       <c r="X6">
-        <v>6.6533869360029918E-2</v>
+        <v>-4.7357994610160922E-3</v>
       </c>
       <c r="Y6">
-        <v>-1.6183289520876366E-3</v>
+        <v>4.3020456196813891E-5</v>
       </c>
       <c r="Z6">
-        <v>-8.0898714982769349E-2</v>
+        <v>-1.652608191150591E-2</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -5947,79 +5947,79 @@
         <v>104</v>
       </c>
       <c r="B7" s="28">
-        <v>-7.2566355467811136E-2</v>
+        <v>5.9755508676466208E-3</v>
       </c>
       <c r="C7">
-        <v>8.8605321813985463E-5</v>
+        <v>1.5719330222309109E-5</v>
       </c>
       <c r="D7">
-        <v>-6.6697943535855135E-7</v>
+        <v>-1.3431323760227534E-7</v>
       </c>
       <c r="E7">
-        <v>2.976442973231429E-5</v>
+        <v>-5.683802682867253E-5</v>
       </c>
       <c r="F7">
-        <v>-1.5507832220929295E-5</v>
+        <v>-6.8083728076814297E-5</v>
       </c>
       <c r="G7">
-        <v>2.9434168276576411E-4</v>
+        <v>8.1688846746337876E-5</v>
       </c>
       <c r="H7">
-        <v>9.4046445689027259E-4</v>
+        <v>2.9992791893470162E-4</v>
       </c>
       <c r="I7">
-        <v>2.3926191059579771E-4</v>
+        <v>9.8633594509752506E-5</v>
       </c>
       <c r="J7">
-        <v>3.5017945303361312E-5</v>
+        <v>1.6395090225673038E-5</v>
       </c>
       <c r="K7">
-        <v>-3.4285267370081588E-6</v>
+        <v>-1.1759938707219662E-5</v>
       </c>
       <c r="L7">
-        <v>3.082069403792455E-5</v>
+        <v>8.1165611471214333E-6</v>
       </c>
       <c r="M7">
-        <v>-3.0994526086088791E-5</v>
+        <v>7.144726033959703E-5</v>
       </c>
       <c r="N7">
-        <v>-2.4083254856631939E-5</v>
+        <v>6.6232437735719686E-5</v>
       </c>
       <c r="O7">
-        <v>2.7243255109180177E-4</v>
+        <v>1.1343554402137819E-4</v>
       </c>
       <c r="P7">
-        <v>1.0969488631573573E-4</v>
+        <v>1.1103298404921977E-4</v>
       </c>
       <c r="Q7">
-        <v>9.2534945371344472E-5</v>
+        <v>8.8462451188262811E-5</v>
       </c>
       <c r="R7">
-        <v>1.6772144338213089E-4</v>
+        <v>1.1876559666307524E-4</v>
       </c>
       <c r="S7">
-        <v>3.291128565794635E-5</v>
+        <v>9.0150629224897876E-5</v>
       </c>
       <c r="T7">
-        <v>1.4007328731863796E-4</v>
+        <v>9.72192446178408E-5</v>
       </c>
       <c r="U7">
-        <v>2.6174130433815777E-5</v>
+        <v>8.5106386090931844E-5</v>
       </c>
       <c r="V7">
-        <v>-7.6026805321881535E-5</v>
+        <v>3.3903209466464739E-5</v>
       </c>
       <c r="W7">
-        <v>-3.9909402333435096E-5</v>
+        <v>5.1258372131232936E-5</v>
       </c>
       <c r="X7">
-        <v>3.5126484628456578E-3</v>
+        <v>2.3614256033634845E-4</v>
       </c>
       <c r="Y7">
-        <v>-8.0380650687744692E-5</v>
+        <v>6.6799869132560012E-7</v>
       </c>
       <c r="Z7">
-        <v>-5.7812707731220436E-3</v>
+        <v>-8.4901995721277379E-4</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -6027,79 +6027,79 @@
         <v>105</v>
       </c>
       <c r="B8" s="28">
-        <v>-0.18696864190856644</v>
+        <v>-2.0195610883445101E-2</v>
       </c>
       <c r="C8">
-        <v>3.7567933403402295E-4</v>
+        <v>1.0424941899692119E-4</v>
       </c>
       <c r="D8">
-        <v>-2.3251328124177905E-6</v>
+        <v>-6.4626443055687164E-7</v>
       </c>
       <c r="E8">
-        <v>2.6728937961888449E-5</v>
+        <v>1.2962781811681138E-5</v>
       </c>
       <c r="F8">
-        <v>-3.4222339019402922E-5</v>
+        <v>-1.4966712754450667E-5</v>
       </c>
       <c r="G8">
-        <v>7.5782904484281849E-4</v>
+        <v>2.4447737503135135E-4</v>
       </c>
       <c r="H8">
-        <v>2.3926191059579771E-4</v>
+        <v>9.8633594509752506E-5</v>
       </c>
       <c r="I8">
-        <v>5.635869284144078E-2</v>
+        <v>3.5919317808059424E-2</v>
       </c>
       <c r="J8">
-        <v>-5.51725964321257E-5</v>
+        <v>-7.2517845450541431E-6</v>
       </c>
       <c r="K8">
-        <v>1.2773057338093767E-5</v>
+        <v>1.3296496444301696E-5</v>
       </c>
       <c r="L8">
-        <v>7.8975305104289715E-5</v>
+        <v>2.3217065626595363E-6</v>
       </c>
       <c r="M8">
-        <v>5.2215717412867869E-4</v>
+        <v>2.4477117041753129E-4</v>
       </c>
       <c r="N8">
-        <v>5.073613785321169E-4</v>
+        <v>2.373408824797059E-4</v>
       </c>
       <c r="O8">
-        <v>2.1641327389217732E-4</v>
+        <v>1.3279589122628445E-4</v>
       </c>
       <c r="P8">
-        <v>6.2695343103707168E-4</v>
+        <v>2.6911297470843295E-4</v>
       </c>
       <c r="Q8">
-        <v>5.4080899331276222E-6</v>
+        <v>8.234721968269798E-6</v>
       </c>
       <c r="R8">
-        <v>4.3589338120417166E-4</v>
+        <v>2.123648566229539E-4</v>
       </c>
       <c r="S8">
-        <v>3.6465310762041556E-4</v>
+        <v>1.8529967265687062E-4</v>
       </c>
       <c r="T8">
-        <v>6.2052294914696055E-4</v>
+        <v>1.9596742889575243E-4</v>
       </c>
       <c r="U8">
-        <v>3.7722166392213652E-4</v>
+        <v>1.9142379002872058E-4</v>
       </c>
       <c r="V8">
-        <v>5.9080020060350489E-4</v>
+        <v>2.4154108930725629E-4</v>
       </c>
       <c r="W8">
-        <v>5.3643715288792266E-4</v>
+        <v>2.0866289437478021E-4</v>
       </c>
       <c r="X8">
-        <v>8.6672616631162103E-3</v>
+        <v>-4.0081121950490354E-3</v>
       </c>
       <c r="Y8">
-        <v>-2.3240115642635725E-4</v>
+        <v>2.719324280039407E-5</v>
       </c>
       <c r="Z8">
-        <v>-2.1087593042925512E-2</v>
+        <v>-8.7856550969237423E-4</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -6107,79 +6107,79 @@
         <v>85</v>
       </c>
       <c r="B9" s="28">
-        <v>5.2705088084751661E-2</v>
+        <v>2.6621479581249399E-2</v>
       </c>
       <c r="C9">
-        <v>-3.2245710373524409E-5</v>
+        <v>-8.6716598173288383E-6</v>
       </c>
       <c r="D9">
-        <v>2.1364090698061375E-7</v>
+        <v>6.0800442814289225E-8</v>
       </c>
       <c r="E9">
-        <v>4.1148245902515316E-5</v>
+        <v>8.0411296576683364E-6</v>
       </c>
       <c r="F9">
-        <v>4.7397751599940414E-5</v>
+        <v>1.479434067412174E-5</v>
       </c>
       <c r="G9">
-        <v>-1.235074849913667E-4</v>
+        <v>-3.3909078767468612E-5</v>
       </c>
       <c r="H9">
-        <v>3.5017945303361312E-5</v>
+        <v>1.6395090225673038E-5</v>
       </c>
       <c r="I9">
-        <v>-5.51725964321257E-5</v>
+        <v>-7.2517845450541431E-6</v>
       </c>
       <c r="J9">
-        <v>1.5147344644291332E-4</v>
+        <v>6.3550293279961351E-5</v>
       </c>
       <c r="K9">
-        <v>-1.1838810542074378E-5</v>
+        <v>-4.0995766540062552E-6</v>
       </c>
       <c r="L9">
-        <v>-2.6901708371575338E-6</v>
+        <v>-9.0550394732067405E-7</v>
       </c>
       <c r="M9">
-        <v>-3.4169738985624346E-6</v>
+        <v>1.7643751806232415E-6</v>
       </c>
       <c r="N9">
-        <v>-3.6473326011718951E-5</v>
+        <v>-4.0427114584778512E-6</v>
       </c>
       <c r="O9">
-        <v>8.5096436023373548E-6</v>
+        <v>-8.8368978520598118E-6</v>
       </c>
       <c r="P9">
-        <v>3.782424155320674E-7</v>
+        <v>-1.2050953682148967E-5</v>
       </c>
       <c r="Q9">
-        <v>-1.284280720018297E-5</v>
+        <v>-8.8250748936773713E-6</v>
       </c>
       <c r="R9">
-        <v>-2.9540570808990886E-7</v>
+        <v>-8.3009028212775341E-6</v>
       </c>
       <c r="S9">
-        <v>-1.0138721929766784E-5</v>
+        <v>-1.2588527064325109E-5</v>
       </c>
       <c r="T9">
-        <v>-7.9356182388963243E-5</v>
+        <v>-3.2013686017522391E-5</v>
       </c>
       <c r="U9">
-        <v>-5.3212278252600179E-5</v>
+        <v>-2.2724384780187294E-5</v>
       </c>
       <c r="V9">
-        <v>-5.1065922562041694E-5</v>
+        <v>-2.1780377932756798E-5</v>
       </c>
       <c r="W9">
-        <v>-4.0359260377752248E-5</v>
+        <v>-2.0977258111140899E-5</v>
       </c>
       <c r="X9">
-        <v>4.0996254422360559E-3</v>
+        <v>-5.5477928704799435E-5</v>
       </c>
       <c r="Y9">
-        <v>-1.0102682383742508E-4</v>
+        <v>2.7488342738027865E-7</v>
       </c>
       <c r="Z9">
-        <v>-1.7892190978239797E-3</v>
+        <v>1.8235667784556901E-4</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -6187,79 +6187,79 @@
         <v>142</v>
       </c>
       <c r="B10" s="28">
-        <v>0.61680425412761564</v>
+        <v>0.65537152015926037</v>
       </c>
       <c r="C10">
-        <v>6.1180726592585557E-5</v>
+        <v>3.5403752053530006E-5</v>
       </c>
       <c r="D10">
-        <v>-3.685521129824482E-7</v>
+        <v>-2.241420469668203E-7</v>
       </c>
       <c r="E10">
-        <v>6.2870510822546805E-5</v>
+        <v>3.4631236955086304E-5</v>
       </c>
       <c r="F10">
-        <v>8.6953927290429141E-5</v>
+        <v>4.7468083932424074E-5</v>
       </c>
       <c r="G10">
-        <v>8.8851347908823746E-7</v>
+        <v>-1.306939603770932E-4</v>
       </c>
       <c r="H10">
-        <v>-3.4285267370081588E-6</v>
+        <v>-1.1759938707219662E-5</v>
       </c>
       <c r="I10">
-        <v>1.2773057338093767E-5</v>
+        <v>1.3296496444301696E-5</v>
       </c>
       <c r="J10">
-        <v>-1.1838810542074378E-5</v>
+        <v>-4.0995766540062552E-6</v>
       </c>
       <c r="K10">
-        <v>2.1407990654368061E-4</v>
+        <v>1.0184588880747084E-4</v>
       </c>
       <c r="L10">
-        <v>-1.8721140499754438E-4</v>
+        <v>-9.3406222938625792E-5</v>
       </c>
       <c r="M10">
-        <v>-8.9657903079333657E-5</v>
+        <v>-7.4824438705388695E-6</v>
       </c>
       <c r="N10">
-        <v>-6.185508414946555E-5</v>
+        <v>-5.9230697481882269E-6</v>
       </c>
       <c r="O10">
-        <v>-9.87140455508091E-5</v>
+        <v>-9.23974099616365E-6</v>
       </c>
       <c r="P10">
-        <v>-5.7486836241456328E-5</v>
+        <v>-1.041649753167515E-5</v>
       </c>
       <c r="Q10">
-        <v>-9.8281067858276686E-5</v>
+        <v>-8.2606710942534838E-6</v>
       </c>
       <c r="R10">
-        <v>-1.0558505241095E-4</v>
+        <v>-1.0273802030676994E-5</v>
       </c>
       <c r="S10">
-        <v>-8.1550807343937204E-5</v>
+        <v>-6.3288289155188232E-6</v>
       </c>
       <c r="T10">
-        <v>-6.2599643884861893E-5</v>
+        <v>-7.2170426823549468E-7</v>
       </c>
       <c r="U10">
-        <v>-5.2945549815373421E-5</v>
+        <v>3.8449775417296911E-6</v>
       </c>
       <c r="V10">
-        <v>-5.8383616800865604E-5</v>
+        <v>-1.5852918890075585E-8</v>
       </c>
       <c r="W10">
-        <v>-4.1852713619102279E-5</v>
+        <v>6.8052853965217095E-6</v>
       </c>
       <c r="X10">
-        <v>1.5104691575832455E-3</v>
+        <v>5.6688264845188149E-5</v>
       </c>
       <c r="Y10">
-        <v>-4.1503688111632696E-5</v>
+        <v>-2.9029480309521257E-6</v>
       </c>
       <c r="Z10">
-        <v>-3.4979352171601516E-3</v>
+        <v>-1.4583407717735641E-3</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -6267,79 +6267,79 @@
         <v>143</v>
       </c>
       <c r="B11" s="28">
-        <v>0.2717489392654942</v>
+        <v>0.25628689773452606</v>
       </c>
       <c r="C11">
-        <v>-2.2895840303450293E-5</v>
+        <v>-2.2090367625242965E-5</v>
       </c>
       <c r="D11">
-        <v>1.2226728446275103E-7</v>
+        <v>1.3693892431078282E-7</v>
       </c>
       <c r="E11">
-        <v>3.4335274356937589E-6</v>
+        <v>-6.2752627584818259E-6</v>
       </c>
       <c r="F11">
-        <v>1.6382202428623648E-5</v>
+        <v>7.6138695030735556E-7</v>
       </c>
       <c r="G11">
-        <v>1.173872549130716E-4</v>
+        <v>1.5446671979272284E-4</v>
       </c>
       <c r="H11">
-        <v>3.082069403792455E-5</v>
+        <v>8.1165611471214333E-6</v>
       </c>
       <c r="I11">
-        <v>7.8975305104289715E-5</v>
+        <v>2.3217065626595363E-6</v>
       </c>
       <c r="J11">
-        <v>-2.6901708371575338E-6</v>
+        <v>-9.0550394732067405E-7</v>
       </c>
       <c r="K11">
-        <v>-1.8721140499754438E-4</v>
+        <v>-9.3406222938625792E-5</v>
       </c>
       <c r="L11">
-        <v>1.9397032488539757E-4</v>
+        <v>9.5657566803527123E-5</v>
       </c>
       <c r="M11">
-        <v>6.4390385134791516E-5</v>
+        <v>7.3751418309950107E-6</v>
       </c>
       <c r="N11">
-        <v>3.9600040446138572E-5</v>
+        <v>2.5281297609119902E-6</v>
       </c>
       <c r="O11">
-        <v>7.9549240594632115E-5</v>
+        <v>1.1503340195538964E-5</v>
       </c>
       <c r="P11">
-        <v>4.2080484503526658E-5</v>
+        <v>1.1489046851286818E-5</v>
       </c>
       <c r="Q11">
-        <v>7.7642066810250406E-5</v>
+        <v>4.6155745327249864E-6</v>
       </c>
       <c r="R11">
-        <v>8.5123306649069992E-5</v>
+        <v>1.0159821491384516E-5</v>
       </c>
       <c r="S11">
-        <v>5.6331749028422308E-5</v>
+        <v>2.519151385421269E-6</v>
       </c>
       <c r="T11">
-        <v>7.0951033153469667E-5</v>
+        <v>6.8660738098925902E-6</v>
       </c>
       <c r="U11">
-        <v>3.4478081438514844E-5</v>
+        <v>-1.6670354725429356E-6</v>
       </c>
       <c r="V11">
-        <v>5.744026542537045E-5</v>
+        <v>3.7799986466636874E-6</v>
       </c>
       <c r="W11">
-        <v>8.4147585510302371E-5</v>
+        <v>8.4024617736883165E-6</v>
       </c>
       <c r="X11">
-        <v>-8.8923418960874107E-4</v>
+        <v>9.1032644968256867E-5</v>
       </c>
       <c r="Y11">
-        <v>2.7276993853721991E-5</v>
+        <v>1.5824406699522373E-6</v>
       </c>
       <c r="Z11">
-        <v>1.3998512112419967E-3</v>
+        <v>7.542878999974665E-4</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -6347,79 +6347,79 @@
         <v>87</v>
       </c>
       <c r="B12" s="28">
-        <v>2.7642724452336748E-2</v>
+        <v>1.9160000662759708E-2</v>
       </c>
       <c r="C12">
-        <v>-9.4592243848465947E-5</v>
+        <v>-1.930560705739031E-5</v>
       </c>
       <c r="D12">
-        <v>5.7887817223021307E-7</v>
+        <v>1.0741127371869533E-7</v>
       </c>
       <c r="E12">
-        <v>-4.4831727718894259E-4</v>
+        <v>-1.8745124017001866E-4</v>
       </c>
       <c r="F12">
-        <v>-3.7610140768106387E-4</v>
+        <v>-1.070704165780817E-4</v>
       </c>
       <c r="G12">
-        <v>-4.2294873251084303E-4</v>
+        <v>-2.0300989717377416E-4</v>
       </c>
       <c r="H12">
-        <v>-3.0994526086088791E-5</v>
+        <v>7.144726033959703E-5</v>
       </c>
       <c r="I12">
-        <v>5.2215717412867869E-4</v>
+        <v>2.4477117041753129E-4</v>
       </c>
       <c r="J12">
-        <v>-3.4169738985624346E-6</v>
+        <v>1.7643751806232415E-6</v>
       </c>
       <c r="K12">
-        <v>-8.9657903079333657E-5</v>
+        <v>-7.4824438705388695E-6</v>
       </c>
       <c r="L12">
-        <v>6.4390385134791516E-5</v>
+        <v>7.3751418309950107E-6</v>
       </c>
       <c r="M12">
-        <v>6.6473658098731804E-3</v>
+        <v>2.8136546432595095E-3</v>
       </c>
       <c r="N12">
-        <v>2.654439685843178E-3</v>
+        <v>1.2747232385644175E-3</v>
       </c>
       <c r="O12">
-        <v>2.6254267222235038E-3</v>
+        <v>1.2746816510595396E-3</v>
       </c>
       <c r="P12">
-        <v>2.6449218518294119E-3</v>
+        <v>1.2847584414855981E-3</v>
       </c>
       <c r="Q12">
-        <v>2.6247497066107222E-3</v>
+        <v>1.2752769216487034E-3</v>
       </c>
       <c r="R12">
-        <v>2.6409006826128593E-3</v>
+        <v>1.2795667523874516E-3</v>
       </c>
       <c r="S12">
-        <v>2.6254807534990634E-3</v>
+        <v>1.2758371177178408E-3</v>
       </c>
       <c r="T12">
-        <v>2.6419154351883375E-3</v>
+        <v>1.2785836447541249E-3</v>
       </c>
       <c r="U12">
-        <v>2.6562086236139319E-3</v>
+        <v>1.2774636358438428E-3</v>
       </c>
       <c r="V12">
-        <v>2.6490854414151148E-3</v>
+        <v>1.2729299311109088E-3</v>
       </c>
       <c r="W12">
-        <v>2.6476074801431238E-3</v>
+        <v>1.2711420661637902E-3</v>
       </c>
       <c r="X12">
-        <v>-1.0451254913843147E-2</v>
+        <v>-1.1293239885466133E-3</v>
       </c>
       <c r="Y12">
-        <v>2.5952268483197226E-4</v>
+        <v>1.9144780041895692E-5</v>
       </c>
       <c r="Z12">
-        <v>8.1918477359313735E-3</v>
+        <v>4.9489536495758539E-4</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -6427,79 +6427,79 @@
         <v>88</v>
       </c>
       <c r="B13" s="28">
-        <v>1.459557696841024E-2</v>
+        <v>2.5228531728485333E-2</v>
       </c>
       <c r="C13">
-        <v>-6.8346612950282923E-5</v>
+        <v>2.0776557835880914E-5</v>
       </c>
       <c r="D13">
-        <v>3.9913128490829598E-7</v>
+        <v>-1.7018896511829257E-7</v>
       </c>
       <c r="E13">
-        <v>-4.2339523174762133E-4</v>
+        <v>-1.876365310173739E-4</v>
       </c>
       <c r="F13">
-        <v>-3.7465494538696493E-4</v>
+        <v>-1.2776670766947616E-4</v>
       </c>
       <c r="G13">
-        <v>-5.219010744585092E-4</v>
+        <v>-1.6478838457802212E-4</v>
       </c>
       <c r="H13">
-        <v>-2.4083254856631939E-5</v>
+        <v>6.6232437735719686E-5</v>
       </c>
       <c r="I13">
-        <v>5.073613785321169E-4</v>
+        <v>2.373408824797059E-4</v>
       </c>
       <c r="J13">
-        <v>-3.6473326011718951E-5</v>
+        <v>-4.0427114584778512E-6</v>
       </c>
       <c r="K13">
-        <v>-6.185508414946555E-5</v>
+        <v>-5.9230697481882269E-6</v>
       </c>
       <c r="L13">
-        <v>3.9600040446138572E-5</v>
+        <v>2.5281297609119902E-6</v>
       </c>
       <c r="M13">
-        <v>2.654439685843178E-3</v>
+        <v>1.2747232385644175E-3</v>
       </c>
       <c r="N13">
-        <v>3.9764245050987633E-3</v>
+        <v>1.7762036888703649E-3</v>
       </c>
       <c r="O13">
-        <v>2.6287846812610583E-3</v>
+        <v>1.2722561024018923E-3</v>
       </c>
       <c r="P13">
-        <v>2.6451510875256886E-3</v>
+        <v>1.2792710214422675E-3</v>
       </c>
       <c r="Q13">
-        <v>2.6332814371561523E-3</v>
+        <v>1.2764965337856656E-3</v>
       </c>
       <c r="R13">
-        <v>2.6493377295655654E-3</v>
+        <v>1.280690382363833E-3</v>
       </c>
       <c r="S13">
-        <v>2.6325107613275698E-3</v>
+        <v>1.277927265737219E-3</v>
       </c>
       <c r="T13">
-        <v>2.6557424899618059E-3</v>
+        <v>1.2793908166496793E-3</v>
       </c>
       <c r="U13">
-        <v>2.6664299182177311E-3</v>
+        <v>1.27352148566272E-3</v>
       </c>
       <c r="V13">
-        <v>2.6439402403564015E-3</v>
+        <v>1.2680871898239679E-3</v>
       </c>
       <c r="W13">
-        <v>2.6449435491030064E-3</v>
+        <v>1.2697342983791792E-3</v>
       </c>
       <c r="X13">
-        <v>1.2567800871521498E-2</v>
+        <v>-1.886234748059149E-3</v>
       </c>
       <c r="Y13">
-        <v>-2.7231207255908182E-4</v>
+        <v>2.2101038271362029E-5</v>
       </c>
       <c r="Z13">
-        <v>-7.6671426464842915E-3</v>
+        <v>-1.77369653603595E-4</v>
       </c>
     </row>
     <row r="14" spans="1:26">
@@ -6507,79 +6507,79 @@
         <v>89</v>
       </c>
       <c r="B14" s="28">
-        <v>1.2831842284793647E-2</v>
+        <v>-3.1648876356366895E-3</v>
       </c>
       <c r="C14">
-        <v>-2.6691493729107639E-5</v>
+        <v>-1.2147216036976181E-6</v>
       </c>
       <c r="D14">
-        <v>8.1953104917087177E-8</v>
+        <v>-3.6363855614194652E-8</v>
       </c>
       <c r="E14">
-        <v>-2.5770843396612236E-4</v>
+        <v>-1.388882832725449E-4</v>
       </c>
       <c r="F14">
-        <v>-3.1174040395174816E-4</v>
+        <v>-8.9296990456226902E-5</v>
       </c>
       <c r="G14">
-        <v>-2.8911914461411171E-4</v>
+        <v>-9.2479255672741571E-5</v>
       </c>
       <c r="H14">
-        <v>2.7243255109180177E-4</v>
+        <v>1.1343554402137819E-4</v>
       </c>
       <c r="I14">
-        <v>2.1641327389217732E-4</v>
+        <v>1.3279589122628445E-4</v>
       </c>
       <c r="J14">
-        <v>8.5096436023373548E-6</v>
+        <v>-8.8368978520598118E-6</v>
       </c>
       <c r="K14">
-        <v>-9.87140455508091E-5</v>
+        <v>-9.23974099616365E-6</v>
       </c>
       <c r="L14">
-        <v>7.9549240594632115E-5</v>
+        <v>1.1503340195538964E-5</v>
       </c>
       <c r="M14">
-        <v>2.6254267222235038E-3</v>
+        <v>1.2746816510595396E-3</v>
       </c>
       <c r="N14">
-        <v>2.6287846812610583E-3</v>
+        <v>1.2722561024018923E-3</v>
       </c>
       <c r="O14">
-        <v>4.7547022520887097E-3</v>
+        <v>2.0545860429161027E-3</v>
       </c>
       <c r="P14">
-        <v>2.6280447427469399E-3</v>
+        <v>1.2858175754855697E-3</v>
       </c>
       <c r="Q14">
-        <v>2.6463070973605073E-3</v>
+        <v>1.2821835417323186E-3</v>
       </c>
       <c r="R14">
-        <v>2.6651628306459743E-3</v>
+        <v>1.2907019138037176E-3</v>
       </c>
       <c r="S14">
-        <v>2.6310546785295566E-3</v>
+        <v>1.2829592165665342E-3</v>
       </c>
       <c r="T14">
-        <v>2.6585430190041635E-3</v>
+        <v>1.2900912751364719E-3</v>
       </c>
       <c r="U14">
-        <v>2.6536904009532227E-3</v>
+        <v>1.2812363158923364E-3</v>
       </c>
       <c r="V14">
-        <v>2.6060909217077021E-3</v>
+        <v>1.2679818904691434E-3</v>
       </c>
       <c r="W14">
-        <v>2.5916544104670008E-3</v>
+        <v>1.2711100495833945E-3</v>
       </c>
       <c r="X14">
-        <v>9.8335438760414756E-3</v>
+        <v>-1.1151911571332133E-3</v>
       </c>
       <c r="Y14">
-        <v>-2.3746763530111314E-4</v>
+        <v>1.4071687890389447E-5</v>
       </c>
       <c r="Z14">
-        <v>-7.1245336240059985E-3</v>
+        <v>-1.4315450701872512E-5</v>
       </c>
     </row>
     <row r="15" spans="1:26">
@@ -6587,79 +6587,79 @@
         <v>90</v>
       </c>
       <c r="B15" s="28">
-        <v>3.9903506549119401E-2</v>
+        <v>4.4949200228131252E-2</v>
       </c>
       <c r="C15">
-        <v>5.9759702456547732E-5</v>
+        <v>4.2734456843327058E-5</v>
       </c>
       <c r="D15">
-        <v>-4.2092067576003186E-7</v>
+        <v>-3.1098703171011699E-7</v>
       </c>
       <c r="E15">
-        <v>-3.6790244928033345E-4</v>
+        <v>-1.6192015913526063E-4</v>
       </c>
       <c r="F15">
-        <v>-3.7918439509132188E-4</v>
+        <v>-1.1659716042343161E-4</v>
       </c>
       <c r="G15">
-        <v>-3.9753732376365597E-4</v>
+        <v>-1.3168394035841056E-4</v>
       </c>
       <c r="H15">
-        <v>1.0969488631573573E-4</v>
+        <v>1.1103298404921977E-4</v>
       </c>
       <c r="I15">
-        <v>6.2695343103707168E-4</v>
+        <v>2.6911297470843295E-4</v>
       </c>
       <c r="J15">
-        <v>3.782424155320674E-7</v>
+        <v>-1.2050953682148967E-5</v>
       </c>
       <c r="K15">
-        <v>-5.7486836241456328E-5</v>
+        <v>-1.041649753167515E-5</v>
       </c>
       <c r="L15">
-        <v>4.2080484503526658E-5</v>
+        <v>1.1489046851286818E-5</v>
       </c>
       <c r="M15">
-        <v>2.6449218518294119E-3</v>
+        <v>1.2847584414855981E-3</v>
       </c>
       <c r="N15">
-        <v>2.6451510875256886E-3</v>
+        <v>1.2792710214422675E-3</v>
       </c>
       <c r="O15">
-        <v>2.6280447427469399E-3</v>
+        <v>1.2858175754855697E-3</v>
       </c>
       <c r="P15">
-        <v>4.6119371808255802E-3</v>
+        <v>2.0995407388755432E-3</v>
       </c>
       <c r="Q15">
-        <v>2.6325856371116254E-3</v>
+        <v>1.2854576060014073E-3</v>
       </c>
       <c r="R15">
-        <v>2.6343596565110831E-3</v>
+        <v>1.2935452678582676E-3</v>
       </c>
       <c r="S15">
-        <v>2.6056111389355209E-3</v>
+        <v>1.2824948509833321E-3</v>
       </c>
       <c r="T15">
-        <v>2.6479491512437815E-3</v>
+        <v>1.2917585042210122E-3</v>
       </c>
       <c r="U15">
-        <v>2.6509758552934262E-3</v>
+        <v>1.2856243947140895E-3</v>
       </c>
       <c r="V15">
-        <v>2.6223897143918258E-3</v>
+        <v>1.2729982577080723E-3</v>
       </c>
       <c r="W15">
-        <v>2.6191334915695707E-3</v>
+        <v>1.2717993055643161E-3</v>
       </c>
       <c r="X15">
-        <v>2.1833653367780224E-2</v>
+        <v>-1.9825766725243762E-4</v>
       </c>
       <c r="Y15">
-        <v>-5.3263120264350494E-4</v>
+        <v>-2.2811395067371364E-6</v>
       </c>
       <c r="Z15">
-        <v>-1.8161477096303245E-2</v>
+        <v>-2.3843492695452811E-3</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -6667,79 +6667,79 @@
         <v>91</v>
       </c>
       <c r="B16" s="28">
-        <v>1.2395415091484669E-2</v>
+        <v>2.7336824544160001E-2</v>
       </c>
       <c r="C16">
-        <v>-3.2262003646115118E-6</v>
+        <v>1.0399314842201701E-5</v>
       </c>
       <c r="D16">
-        <v>-5.3535383524400343E-9</v>
+        <v>-1.0083302118018867E-7</v>
       </c>
       <c r="E16">
-        <v>-3.051954617120086E-4</v>
+        <v>-1.5434046213837145E-4</v>
       </c>
       <c r="F16">
-        <v>-3.8023980269021436E-4</v>
+        <v>-1.4844482791552904E-4</v>
       </c>
       <c r="G16">
-        <v>9.8221918369822985E-5</v>
+        <v>4.5569941411718624E-5</v>
       </c>
       <c r="H16">
-        <v>9.2534945371344472E-5</v>
+        <v>8.8462451188262811E-5</v>
       </c>
       <c r="I16">
-        <v>5.4080899331276222E-6</v>
+        <v>8.234721968269798E-6</v>
       </c>
       <c r="J16">
-        <v>-1.284280720018297E-5</v>
+        <v>-8.8250748936773713E-6</v>
       </c>
       <c r="K16">
-        <v>-9.8281067858276686E-5</v>
+        <v>-8.2606710942534838E-6</v>
       </c>
       <c r="L16">
-        <v>7.7642066810250406E-5</v>
+        <v>4.6155745327249864E-6</v>
       </c>
       <c r="M16">
-        <v>2.6247497066107222E-3</v>
+        <v>1.2752769216487034E-3</v>
       </c>
       <c r="N16">
-        <v>2.6332814371561523E-3</v>
+        <v>1.2764965337856656E-3</v>
       </c>
       <c r="O16">
-        <v>2.6463070973605073E-3</v>
+        <v>1.2821835417323186E-3</v>
       </c>
       <c r="P16">
-        <v>2.6325856371116254E-3</v>
+        <v>1.2854576060014073E-3</v>
       </c>
       <c r="Q16">
-        <v>4.5578497217168808E-3</v>
+        <v>2.0671190642478445E-3</v>
       </c>
       <c r="R16">
-        <v>2.6404531392171977E-3</v>
+        <v>1.2897431222816556E-3</v>
       </c>
       <c r="S16">
-        <v>2.610087518325538E-3</v>
+        <v>1.2816454883691104E-3</v>
       </c>
       <c r="T16">
-        <v>2.6455616966002404E-3</v>
+        <v>1.2884484293289411E-3</v>
       </c>
       <c r="U16">
-        <v>2.6503836417729265E-3</v>
+        <v>1.2848187115470961E-3</v>
       </c>
       <c r="V16">
-        <v>2.6187660781863166E-3</v>
+        <v>1.2704388648209076E-3</v>
       </c>
       <c r="W16">
-        <v>2.6351988479916921E-3</v>
+        <v>1.2776763467245164E-3</v>
       </c>
       <c r="X16">
-        <v>-6.4315501130817465E-3</v>
+        <v>-5.7763825988162674E-4</v>
       </c>
       <c r="Y16">
-        <v>1.6912574526897848E-4</v>
+        <v>1.5397412843357009E-5</v>
       </c>
       <c r="Z16">
-        <v>1.9419798406235117E-3</v>
+        <v>-1.0010339781156077E-3</v>
       </c>
     </row>
     <row r="17" spans="1:26">
@@ -6747,79 +6747,79 @@
         <v>92</v>
       </c>
       <c r="B17" s="28">
-        <v>8.0298242159205571E-2</v>
+        <v>3.5872517731070939E-2</v>
       </c>
       <c r="C17">
-        <v>-6.5930193543487729E-5</v>
+        <v>2.0409188832499862E-5</v>
       </c>
       <c r="D17">
-        <v>3.3827118408761908E-7</v>
+        <v>-1.8965834056824574E-7</v>
       </c>
       <c r="E17">
-        <v>-2.6714371800515171E-4</v>
+        <v>-1.3706720043480102E-4</v>
       </c>
       <c r="F17">
-        <v>-2.7823869007108717E-4</v>
+        <v>-1.0247255024790043E-4</v>
       </c>
       <c r="G17">
-        <v>-2.6180768963694019E-4</v>
+        <v>-1.1988575043978423E-4</v>
       </c>
       <c r="H17">
-        <v>1.6772144338213089E-4</v>
+        <v>1.1876559666307524E-4</v>
       </c>
       <c r="I17">
-        <v>4.3589338120417166E-4</v>
+        <v>2.123648566229539E-4</v>
       </c>
       <c r="J17">
-        <v>-2.9540570808990886E-7</v>
+        <v>-8.3009028212775341E-6</v>
       </c>
       <c r="K17">
-        <v>-1.0558505241095E-4</v>
+        <v>-1.0273802030676994E-5</v>
       </c>
       <c r="L17">
-        <v>8.5123306649069992E-5</v>
+        <v>1.0159821491384516E-5</v>
       </c>
       <c r="M17">
-        <v>2.6409006826128593E-3</v>
+        <v>1.2795667523874516E-3</v>
       </c>
       <c r="N17">
-        <v>2.6493377295655654E-3</v>
+        <v>1.280690382363833E-3</v>
       </c>
       <c r="O17">
-        <v>2.6651628306459743E-3</v>
+        <v>1.2907019138037176E-3</v>
       </c>
       <c r="P17">
-        <v>2.6343596565110831E-3</v>
+        <v>1.2935452678582676E-3</v>
       </c>
       <c r="Q17">
-        <v>2.6404531392171977E-3</v>
+        <v>1.2897431222816556E-3</v>
       </c>
       <c r="R17">
-        <v>4.0126630432356794E-3</v>
+        <v>1.8989830942598594E-3</v>
       </c>
       <c r="S17">
-        <v>2.6413684650881935E-3</v>
+        <v>1.289657467889013E-3</v>
       </c>
       <c r="T17">
-        <v>2.6681200716919735E-3</v>
+        <v>1.3002740782589802E-3</v>
       </c>
       <c r="U17">
-        <v>2.6716879420479686E-3</v>
+        <v>1.2923413244039028E-3</v>
       </c>
       <c r="V17">
-        <v>2.6186039950588467E-3</v>
+        <v>1.2732193854143366E-3</v>
       </c>
       <c r="W17">
-        <v>2.6249131131433519E-3</v>
+        <v>1.2826559554233526E-3</v>
       </c>
       <c r="X17">
-        <v>7.7752173871977609E-4</v>
+        <v>-8.7096158698655567E-4</v>
       </c>
       <c r="Y17">
-        <v>2.5717771938350668E-5</v>
+        <v>1.8055537645629517E-5</v>
       </c>
       <c r="Z17">
-        <v>-4.7579455731514703E-4</v>
+        <v>-1.062587737781142E-3</v>
       </c>
     </row>
     <row r="18" spans="1:26">
@@ -6827,79 +6827,79 @@
         <v>93</v>
       </c>
       <c r="B18" s="28">
-        <v>5.5214611779628643E-2</v>
+        <v>5.2913657515805131E-2</v>
       </c>
       <c r="C18">
-        <v>-4.2587369656575495E-5</v>
+        <v>2.3163108354805687E-5</v>
       </c>
       <c r="D18">
-        <v>2.0682632061465967E-7</v>
+        <v>-1.9136278392855455E-7</v>
       </c>
       <c r="E18">
-        <v>-2.6152777635922767E-4</v>
+        <v>-1.2633399493739594E-4</v>
       </c>
       <c r="F18">
-        <v>-2.6774173849786588E-4</v>
+        <v>-8.5871971464446272E-5</v>
       </c>
       <c r="G18">
-        <v>1.8355622887480591E-6</v>
+        <v>3.6849710356013157E-4</v>
       </c>
       <c r="H18">
-        <v>3.291128565794635E-5</v>
+        <v>9.0150629224897876E-5</v>
       </c>
       <c r="I18">
-        <v>3.6465310762041556E-4</v>
+        <v>1.8529967265687062E-4</v>
       </c>
       <c r="J18">
-        <v>-1.0138721929766784E-5</v>
+        <v>-1.2588527064325109E-5</v>
       </c>
       <c r="K18">
-        <v>-8.1550807343937204E-5</v>
+        <v>-6.3288289155188232E-6</v>
       </c>
       <c r="L18">
-        <v>5.6331749028422308E-5</v>
+        <v>2.519151385421269E-6</v>
       </c>
       <c r="M18">
-        <v>2.6254807534990634E-3</v>
+        <v>1.2758371177178408E-3</v>
       </c>
       <c r="N18">
-        <v>2.6325107613275698E-3</v>
+        <v>1.277927265737219E-3</v>
       </c>
       <c r="O18">
-        <v>2.6310546785295566E-3</v>
+        <v>1.2829592165665342E-3</v>
       </c>
       <c r="P18">
-        <v>2.6056111389355209E-3</v>
+        <v>1.2824948509833321E-3</v>
       </c>
       <c r="Q18">
-        <v>2.610087518325538E-3</v>
+        <v>1.2816454883691104E-3</v>
       </c>
       <c r="R18">
-        <v>2.6413684650881935E-3</v>
+        <v>1.289657467889013E-3</v>
       </c>
       <c r="S18">
-        <v>3.4318573789728938E-3</v>
+        <v>1.6750439536085814E-3</v>
       </c>
       <c r="T18">
-        <v>2.6296704584651302E-3</v>
+        <v>1.2908864345565138E-3</v>
       </c>
       <c r="U18">
-        <v>2.6417992212542348E-3</v>
+        <v>1.2852346285027738E-3</v>
       </c>
       <c r="V18">
-        <v>2.5970153866153346E-3</v>
+        <v>1.2689813994242152E-3</v>
       </c>
       <c r="W18">
-        <v>2.5849177784297147E-3</v>
+        <v>1.266637403253233E-3</v>
       </c>
       <c r="X18">
-        <v>1.7791963511890843E-2</v>
+        <v>-2.3334016108239857E-4</v>
       </c>
       <c r="Y18">
-        <v>-4.075143993274867E-4</v>
+        <v>9.9044575108987054E-6</v>
       </c>
       <c r="Z18">
-        <v>-1.1854937581493821E-2</v>
+        <v>-1.7351826875859899E-3</v>
       </c>
     </row>
     <row r="19" spans="1:26">
@@ -6907,79 +6907,79 @@
         <v>94</v>
       </c>
       <c r="B19" s="28">
-        <v>-6.5251401569957707E-2</v>
+        <v>-2.3685383254163722E-2</v>
       </c>
       <c r="C19">
-        <v>6.5819183852231129E-5</v>
+        <v>3.7923589918188554E-5</v>
       </c>
       <c r="D19">
-        <v>-5.1410633012882669E-7</v>
+        <v>-3.0076477070616167E-7</v>
       </c>
       <c r="E19">
-        <v>-3.6172391422070857E-4</v>
+        <v>-1.2890844974696255E-4</v>
       </c>
       <c r="F19">
-        <v>-2.9718166205165047E-4</v>
+        <v>-6.9829062721032292E-5</v>
       </c>
       <c r="G19">
-        <v>-7.875914842202323E-5</v>
+        <v>-6.9678050691199603E-6</v>
       </c>
       <c r="H19">
-        <v>1.4007328731863796E-4</v>
+        <v>9.72192446178408E-5</v>
       </c>
       <c r="I19">
-        <v>6.2052294914696055E-4</v>
+        <v>1.9596742889575243E-4</v>
       </c>
       <c r="J19">
-        <v>-7.9356182388963243E-5</v>
+        <v>-3.2013686017522391E-5</v>
       </c>
       <c r="K19">
-        <v>-6.2599643884861893E-5</v>
+        <v>-7.2170426823549468E-7</v>
       </c>
       <c r="L19">
-        <v>7.0951033153469667E-5</v>
+        <v>6.8660738098925902E-6</v>
       </c>
       <c r="M19">
-        <v>2.6419154351883375E-3</v>
+        <v>1.2785836447541249E-3</v>
       </c>
       <c r="N19">
-        <v>2.6557424899618059E-3</v>
+        <v>1.2793908166496793E-3</v>
       </c>
       <c r="O19">
-        <v>2.6585430190041635E-3</v>
+        <v>1.2900912751364719E-3</v>
       </c>
       <c r="P19">
-        <v>2.6479491512437815E-3</v>
+        <v>1.2917585042210122E-3</v>
       </c>
       <c r="Q19">
-        <v>2.6455616966002404E-3</v>
+        <v>1.2884484293289411E-3</v>
       </c>
       <c r="R19">
-        <v>2.6681200716919735E-3</v>
+        <v>1.3002740782589802E-3</v>
       </c>
       <c r="S19">
-        <v>2.6296704584651302E-3</v>
+        <v>1.2908864345565138E-3</v>
       </c>
       <c r="T19">
-        <v>4.0863607473623029E-3</v>
+        <v>1.8166905222922122E-3</v>
       </c>
       <c r="U19">
-        <v>2.6847618472817343E-3</v>
+        <v>1.2948604453829607E-3</v>
       </c>
       <c r="V19">
-        <v>2.6358439184560353E-3</v>
+        <v>1.2764512615071127E-3</v>
       </c>
       <c r="W19">
-        <v>2.6736193353142741E-3</v>
+        <v>1.2859520114838318E-3</v>
       </c>
       <c r="X19">
-        <v>4.0115502950429649E-3</v>
+        <v>-5.7022719518375065E-4</v>
       </c>
       <c r="Y19">
-        <v>-6.530418303036167E-5</v>
+        <v>1.5484375792938572E-5</v>
       </c>
       <c r="Z19">
-        <v>-7.2509743736137583E-3</v>
+        <v>-1.9720825112908083E-3</v>
       </c>
     </row>
     <row r="20" spans="1:26">
@@ -6987,79 +6987,79 @@
         <v>95</v>
       </c>
       <c r="B20" s="28">
-        <v>8.0250868006236209E-2</v>
+        <v>2.1714981492603324E-2</v>
       </c>
       <c r="C20">
-        <v>-9.1381558844600558E-5</v>
+        <v>-5.7459094906387592E-6</v>
       </c>
       <c r="D20">
-        <v>5.4238921900210324E-7</v>
+        <v>-3.139509319576299E-9</v>
       </c>
       <c r="E20">
-        <v>-4.2923649245604599E-4</v>
+        <v>-1.7128649949495859E-4</v>
       </c>
       <c r="F20">
-        <v>-4.5650319825589405E-4</v>
+        <v>-1.2778979179038668E-4</v>
       </c>
       <c r="G20">
-        <v>-2.9133596961072438E-4</v>
+        <v>-4.8048469678683287E-5</v>
       </c>
       <c r="H20">
-        <v>2.6174130433815777E-5</v>
+        <v>8.5106386090931844E-5</v>
       </c>
       <c r="I20">
-        <v>3.7722166392213652E-4</v>
+        <v>1.9142379002872058E-4</v>
       </c>
       <c r="J20">
-        <v>-5.3212278252600179E-5</v>
+        <v>-2.2724384780187294E-5</v>
       </c>
       <c r="K20">
-        <v>-5.2945549815373421E-5</v>
+        <v>3.8449775417296911E-6</v>
       </c>
       <c r="L20">
-        <v>3.4478081438514844E-5</v>
+        <v>-1.6670354725429356E-6</v>
       </c>
       <c r="M20">
-        <v>2.6562086236139319E-3</v>
+        <v>1.2774636358438428E-3</v>
       </c>
       <c r="N20">
-        <v>2.6664299182177311E-3</v>
+        <v>1.27352148566272E-3</v>
       </c>
       <c r="O20">
-        <v>2.6536904009532227E-3</v>
+        <v>1.2812363158923364E-3</v>
       </c>
       <c r="P20">
-        <v>2.6509758552934262E-3</v>
+        <v>1.2856243947140895E-3</v>
       </c>
       <c r="Q20">
-        <v>2.6503836417729265E-3</v>
+        <v>1.2848187115470961E-3</v>
       </c>
       <c r="R20">
-        <v>2.6716879420479686E-3</v>
+        <v>1.2923413244039028E-3</v>
       </c>
       <c r="S20">
-        <v>2.6417992212542348E-3</v>
+        <v>1.2852346285027738E-3</v>
       </c>
       <c r="T20">
-        <v>2.6847618472817343E-3</v>
+        <v>1.2948604453829607E-3</v>
       </c>
       <c r="U20">
-        <v>6.1887269403897976E-3</v>
+        <v>2.545015229810578E-3</v>
       </c>
       <c r="V20">
-        <v>2.643132909646241E-3</v>
+        <v>1.2712402697984179E-3</v>
       </c>
       <c r="W20">
-        <v>2.6398905192997948E-3</v>
+        <v>1.2785104075294304E-3</v>
       </c>
       <c r="X20">
-        <v>1.6274634834936227E-2</v>
+        <v>-1.1298146034274389E-3</v>
       </c>
       <c r="Y20">
-        <v>-3.7623487747610179E-4</v>
+        <v>2.0155845837643022E-5</v>
       </c>
       <c r="Z20">
-        <v>-8.8560459482517305E-3</v>
+        <v>1.4559113904160856E-4</v>
       </c>
     </row>
     <row r="21" spans="1:26">
@@ -7067,79 +7067,79 @@
         <v>96</v>
       </c>
       <c r="B21" s="28">
-        <v>-2.3403708069883494E-2</v>
+        <v>-1.1719138980812076E-2</v>
       </c>
       <c r="C21">
-        <v>1.8962509263316385E-5</v>
+        <v>2.4339083856935242E-5</v>
       </c>
       <c r="D21">
-        <v>-1.4517630199039434E-7</v>
+        <v>-1.8219952600717935E-7</v>
       </c>
       <c r="E21">
-        <v>-3.2635754230038108E-4</v>
+        <v>-1.3350623327530031E-4</v>
       </c>
       <c r="F21">
-        <v>-2.9998103400542082E-4</v>
+        <v>-8.7746162073782519E-5</v>
       </c>
       <c r="G21">
-        <v>-3.265505256146873E-4</v>
+        <v>-1.3279619219293704E-4</v>
       </c>
       <c r="H21">
-        <v>-7.6026805321881535E-5</v>
+        <v>3.3903209466464739E-5</v>
       </c>
       <c r="I21">
-        <v>5.9080020060350489E-4</v>
+        <v>2.4154108930725629E-4</v>
       </c>
       <c r="J21">
-        <v>-5.1065922562041694E-5</v>
+        <v>-2.1780377932756798E-5</v>
       </c>
       <c r="K21">
-        <v>-5.8383616800865604E-5</v>
+        <v>-1.5852918890075585E-8</v>
       </c>
       <c r="L21">
-        <v>5.744026542537045E-5</v>
+        <v>3.7799986466636874E-6</v>
       </c>
       <c r="M21">
-        <v>2.6490854414151148E-3</v>
+        <v>1.2729299311109088E-3</v>
       </c>
       <c r="N21">
-        <v>2.6439402403564015E-3</v>
+        <v>1.2680871898239679E-3</v>
       </c>
       <c r="O21">
-        <v>2.6060909217077021E-3</v>
+        <v>1.2679818904691434E-3</v>
       </c>
       <c r="P21">
-        <v>2.6223897143918258E-3</v>
+        <v>1.2729982577080723E-3</v>
       </c>
       <c r="Q21">
-        <v>2.6187660781863166E-3</v>
+        <v>1.2704388648209076E-3</v>
       </c>
       <c r="R21">
-        <v>2.6186039950588467E-3</v>
+        <v>1.2732193854143366E-3</v>
       </c>
       <c r="S21">
-        <v>2.5970153866153346E-3</v>
+        <v>1.2689813994242152E-3</v>
       </c>
       <c r="T21">
-        <v>2.6358439184560353E-3</v>
+        <v>1.2764512615071127E-3</v>
       </c>
       <c r="U21">
-        <v>2.643132909646241E-3</v>
+        <v>1.2712402697984179E-3</v>
       </c>
       <c r="V21">
-        <v>4.7303818924698659E-3</v>
+        <v>2.1590200609572646E-3</v>
       </c>
       <c r="W21">
-        <v>2.6613174163649909E-3</v>
+        <v>1.272381584671652E-3</v>
       </c>
       <c r="X21">
-        <v>1.4503434485158805E-3</v>
+        <v>-7.3136048555891894E-4</v>
       </c>
       <c r="Y21">
-        <v>-1.7999547177687859E-5</v>
+        <v>1.5262593487825403E-5</v>
       </c>
       <c r="Z21">
-        <v>-3.9325540481387304E-3</v>
+        <v>-1.4217296184754896E-3</v>
       </c>
     </row>
     <row r="22" spans="1:26">
@@ -7147,159 +7147,159 @@
         <v>97</v>
       </c>
       <c r="B22" s="28">
-        <v>-0.12263826410131227</v>
+        <v>-4.995447673226288E-2</v>
       </c>
       <c r="C22">
-        <v>1.0291523765571312E-4</v>
+        <v>4.7464694847966157E-5</v>
       </c>
       <c r="D22">
-        <v>-6.8812246098283263E-7</v>
+        <v>-3.456040478281387E-7</v>
       </c>
       <c r="E22">
-        <v>-3.0472378371160604E-4</v>
+        <v>-1.1696938037380653E-4</v>
       </c>
       <c r="F22">
-        <v>-3.4162095096205753E-4</v>
+        <v>-8.2532978349576227E-5</v>
       </c>
       <c r="G22">
-        <v>-2.9387536816245438E-4</v>
+        <v>-1.7427317757796705E-4</v>
       </c>
       <c r="H22">
-        <v>-3.9909402333435096E-5</v>
+        <v>5.1258372131232936E-5</v>
       </c>
       <c r="I22">
-        <v>5.3643715288792266E-4</v>
+        <v>2.0866289437478021E-4</v>
       </c>
       <c r="J22">
-        <v>-4.0359260377752248E-5</v>
+        <v>-2.0977258111140899E-5</v>
       </c>
       <c r="K22">
-        <v>-4.1852713619102279E-5</v>
+        <v>6.8052853965217095E-6</v>
       </c>
       <c r="L22">
-        <v>8.4147585510302371E-5</v>
+        <v>8.4024617736883165E-6</v>
       </c>
       <c r="M22">
-        <v>2.6476074801431238E-3</v>
+        <v>1.2711420661637902E-3</v>
       </c>
       <c r="N22">
-        <v>2.6449435491030064E-3</v>
+        <v>1.2697342983791792E-3</v>
       </c>
       <c r="O22">
-        <v>2.5916544104670008E-3</v>
+        <v>1.2711100495833945E-3</v>
       </c>
       <c r="P22">
-        <v>2.6191334915695707E-3</v>
+        <v>1.2717993055643161E-3</v>
       </c>
       <c r="Q22">
-        <v>2.6351988479916921E-3</v>
+        <v>1.2776763467245164E-3</v>
       </c>
       <c r="R22">
-        <v>2.6249131131433519E-3</v>
+        <v>1.2826559554233526E-3</v>
       </c>
       <c r="S22">
-        <v>2.5849177784297147E-3</v>
+        <v>1.266637403253233E-3</v>
       </c>
       <c r="T22">
-        <v>2.6736193353142741E-3</v>
+        <v>1.2859520114838318E-3</v>
       </c>
       <c r="U22">
-        <v>2.6398905192997948E-3</v>
+        <v>1.2785104075294304E-3</v>
       </c>
       <c r="V22">
-        <v>2.6613174163649909E-3</v>
+        <v>1.272381584671652E-3</v>
       </c>
       <c r="W22">
-        <v>6.5374332700991874E-3</v>
+        <v>2.879957180437747E-3</v>
       </c>
       <c r="X22">
-        <v>-8.0078014539195497E-3</v>
+        <v>-3.8727743753427268E-3</v>
       </c>
       <c r="Y22">
-        <v>2.4321119376855341E-4</v>
+        <v>5.4710187630284434E-5</v>
       </c>
       <c r="Z22">
-        <v>-1.8934768328584539E-3</v>
+        <v>2.4365859235768212E-4</v>
       </c>
     </row>
     <row r="23" spans="1:26">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B23" s="28">
-        <v>1.8931127459031369</v>
+        <v>-0.42427894801872817</v>
       </c>
       <c r="C23">
-        <v>-2.3516350996442004E-3</v>
+        <v>-6.5626493354240673E-4</v>
       </c>
       <c r="D23">
-        <v>1.3761519885148107E-5</v>
+        <v>4.8721450278470485E-6</v>
       </c>
       <c r="E23">
-        <v>3.1598423342782539E-3</v>
+        <v>1.3172606675703532E-3</v>
       </c>
       <c r="F23">
-        <v>1.6806629907650285E-2</v>
+        <v>1.2650437214488245E-3</v>
       </c>
       <c r="G23">
-        <v>6.6533869360029918E-2</v>
+        <v>-4.7357994610160922E-3</v>
       </c>
       <c r="H23">
-        <v>3.5126484628456578E-3</v>
+        <v>2.3614256033634845E-4</v>
       </c>
       <c r="I23">
-        <v>8.6672616631162103E-3</v>
+        <v>-4.0081121950490354E-3</v>
       </c>
       <c r="J23">
-        <v>4.0996254422360559E-3</v>
+        <v>-5.5477928704799435E-5</v>
       </c>
       <c r="K23">
-        <v>1.5104691575832455E-3</v>
+        <v>5.6688264845188149E-5</v>
       </c>
       <c r="L23">
-        <v>-8.8923418960874107E-4</v>
+        <v>9.1032644968256867E-5</v>
       </c>
       <c r="M23">
-        <v>-1.0451254913843147E-2</v>
+        <v>-1.1293239885466133E-3</v>
       </c>
       <c r="N23">
-        <v>1.2567800871521498E-2</v>
+        <v>-1.886234748059149E-3</v>
       </c>
       <c r="O23">
-        <v>9.8335438760414756E-3</v>
+        <v>-1.1151911571332133E-3</v>
       </c>
       <c r="P23">
-        <v>2.1833653367780224E-2</v>
+        <v>-1.9825766725243762E-4</v>
       </c>
       <c r="Q23">
-        <v>-6.4315501130817465E-3</v>
+        <v>-5.7763825988162674E-4</v>
       </c>
       <c r="R23">
-        <v>7.7752173871977609E-4</v>
+        <v>-8.7096158698655567E-4</v>
       </c>
       <c r="S23">
-        <v>1.7791963511890843E-2</v>
+        <v>-2.3334016108239857E-4</v>
       </c>
       <c r="T23">
-        <v>4.0115502950429649E-3</v>
+        <v>-5.7022719518375065E-4</v>
       </c>
       <c r="U23">
-        <v>1.6274634834936227E-2</v>
+        <v>-1.1298146034274389E-3</v>
       </c>
       <c r="V23">
-        <v>1.4503434485158805E-3</v>
+        <v>-7.3136048555891894E-4</v>
       </c>
       <c r="W23">
-        <v>-8.0078014539195497E-3</v>
+        <v>-3.8727743753427268E-3</v>
       </c>
       <c r="X23">
-        <v>42.907615663247952</v>
+        <v>1.0147594088171559</v>
       </c>
       <c r="Y23">
-        <v>-1.0364961100669881</v>
+        <v>-8.837216263888073E-3</v>
       </c>
       <c r="Z23">
-        <v>-27.223383196415966</v>
+        <v>-0.86030600057425666</v>
       </c>
     </row>
     <row r="24" spans="1:26">
@@ -7307,79 +7307,79 @@
         <v>141</v>
       </c>
       <c r="B24" s="28">
-        <v>-5.9995388716100585E-2</v>
+        <v>-5.6670609689074081E-3</v>
       </c>
       <c r="C24">
-        <v>4.3539395007997223E-5</v>
+        <v>-6.339269094192846E-6</v>
       </c>
       <c r="D24">
-        <v>-2.4952345962033938E-7</v>
+        <v>3.5934411351696912E-8</v>
       </c>
       <c r="E24">
-        <v>-5.7366322052473115E-5</v>
+        <v>-4.6210554317454249E-6</v>
       </c>
       <c r="F24">
-        <v>-3.9249377718462335E-4</v>
+        <v>2.0853709752339351E-7</v>
       </c>
       <c r="G24">
-        <v>-1.6183289520876366E-3</v>
+        <v>4.3020456196813891E-5</v>
       </c>
       <c r="H24">
-        <v>-8.0380650687744692E-5</v>
+        <v>6.6799869132560012E-7</v>
       </c>
       <c r="I24">
-        <v>-2.3240115642635725E-4</v>
+        <v>2.719324280039407E-5</v>
       </c>
       <c r="J24">
-        <v>-1.0102682383742508E-4</v>
+        <v>2.7488342738027865E-7</v>
       </c>
       <c r="K24">
-        <v>-4.1503688111632696E-5</v>
+        <v>-2.9029480309521257E-6</v>
       </c>
       <c r="L24">
-        <v>2.7276993853721991E-5</v>
+        <v>1.5824406699522373E-6</v>
       </c>
       <c r="M24">
-        <v>2.5952268483197226E-4</v>
+        <v>1.9144780041895692E-5</v>
       </c>
       <c r="N24">
-        <v>-2.7231207255908182E-4</v>
+        <v>2.2101038271362029E-5</v>
       </c>
       <c r="O24">
-        <v>-2.3746763530111314E-4</v>
+        <v>1.4071687890389447E-5</v>
       </c>
       <c r="P24">
-        <v>-5.3263120264350494E-4</v>
+        <v>-2.2811395067371364E-6</v>
       </c>
       <c r="Q24">
-        <v>1.6912574526897848E-4</v>
+        <v>1.5397412843357009E-5</v>
       </c>
       <c r="R24">
-        <v>2.5717771938350668E-5</v>
+        <v>1.8055537645629517E-5</v>
       </c>
       <c r="S24">
-        <v>-4.075143993274867E-4</v>
+        <v>9.9044575108987054E-6</v>
       </c>
       <c r="T24">
-        <v>-6.530418303036167E-5</v>
+        <v>1.5484375792938572E-5</v>
       </c>
       <c r="U24">
-        <v>-3.7623487747610179E-4</v>
+        <v>2.0155845837643022E-5</v>
       </c>
       <c r="V24">
-        <v>-1.7999547177687859E-5</v>
+        <v>1.5262593487825403E-5</v>
       </c>
       <c r="W24">
-        <v>2.4321119376855341E-4</v>
+        <v>5.4710187630284434E-5</v>
       </c>
       <c r="X24">
-        <v>-1.0364961100669881</v>
+        <v>-8.837216263888073E-3</v>
       </c>
       <c r="Y24">
-        <v>2.5121488535982284E-2</v>
+        <v>1.1114309776984085E-4</v>
       </c>
       <c r="Z24">
-        <v>0.65689773175701305</v>
+        <v>7.4392522421864449E-3</v>
       </c>
     </row>
     <row r="25" spans="1:26">
@@ -7387,79 +7387,79 @@
         <v>29</v>
       </c>
       <c r="B25" s="28">
-        <v>8.8043292130727249</v>
+        <v>9.0401836405445728</v>
       </c>
       <c r="C25">
-        <v>-3.0139394804159503E-2</v>
+        <v>-1.3954021316085516E-2</v>
       </c>
       <c r="D25">
-        <v>1.9735474045139059E-4</v>
+        <v>9.140888467813529E-5</v>
       </c>
       <c r="E25">
-        <v>-5.0962908247237926E-3</v>
+        <v>-3.590713747542564E-3</v>
       </c>
       <c r="F25">
-        <v>-1.4411966902579655E-2</v>
+        <v>-4.1013676924257798E-3</v>
       </c>
       <c r="G25">
-        <v>-8.0898714982769349E-2</v>
+        <v>-1.652608191150591E-2</v>
       </c>
       <c r="H25">
-        <v>-5.7812707731220436E-3</v>
+        <v>-8.4901995721277379E-4</v>
       </c>
       <c r="I25">
-        <v>-2.1087593042925512E-2</v>
+        <v>-8.7856550969237423E-4</v>
       </c>
       <c r="J25">
-        <v>-1.7892190978239797E-3</v>
+        <v>1.8235667784556901E-4</v>
       </c>
       <c r="K25">
-        <v>-3.4979352171601516E-3</v>
+        <v>-1.4583407717735641E-3</v>
       </c>
       <c r="L25">
-        <v>1.3998512112419967E-3</v>
+        <v>7.542878999974665E-4</v>
       </c>
       <c r="M25">
-        <v>8.1918477359313735E-3</v>
+        <v>4.9489536495758539E-4</v>
       </c>
       <c r="N25">
-        <v>-7.6671426464842915E-3</v>
+        <v>-1.77369653603595E-4</v>
       </c>
       <c r="O25">
-        <v>-7.1245336240059985E-3</v>
+        <v>-1.4315450701872512E-5</v>
       </c>
       <c r="P25">
-        <v>-1.8161477096303245E-2</v>
+        <v>-2.3843492695452811E-3</v>
       </c>
       <c r="Q25">
-        <v>1.9419798406235117E-3</v>
+        <v>-1.0010339781156077E-3</v>
       </c>
       <c r="R25">
-        <v>-4.7579455731514703E-4</v>
+        <v>-1.062587737781142E-3</v>
       </c>
       <c r="S25">
-        <v>-1.1854937581493821E-2</v>
+        <v>-1.7351826875859899E-3</v>
       </c>
       <c r="T25">
-        <v>-7.2509743736137583E-3</v>
+        <v>-1.9720825112908083E-3</v>
       </c>
       <c r="U25">
-        <v>-8.8560459482517305E-3</v>
+        <v>1.4559113904160856E-4</v>
       </c>
       <c r="V25">
-        <v>-3.9325540481387304E-3</v>
+        <v>-1.4217296184754896E-3</v>
       </c>
       <c r="W25">
-        <v>-1.8934768328584539E-3</v>
+        <v>2.4365859235768212E-4</v>
       </c>
       <c r="X25">
-        <v>-27.223383196415966</v>
+        <v>-0.86030600057425666</v>
       </c>
       <c r="Y25">
-        <v>0.65689773175701305</v>
+        <v>7.4392522421864449E-3</v>
       </c>
       <c r="Z25">
-        <v>18.496572735002133</v>
+        <v>1.2821792219973158</v>
       </c>
     </row>
   </sheetData>
@@ -7471,7 +7471,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C2E849-502C-4818-A96C-18EB09FB1CE0}">
   <dimension ref="A1:Y24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -12780,7 +12782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B61645-4A7A-45C4-916C-002E08390D37}">
   <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>